<commit_message>
added target metrics, wrote max_view function
</commit_message>
<xml_diff>
--- a/df_cleaned.xlsx
+++ b/df_cleaned.xlsx
@@ -550,7 +550,7 @@
         <v>166000000</v>
       </c>
       <c r="E4" t="n">
-        <v>-1695929202</v>
+        <v>1695929202</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
         <v>112000000</v>
       </c>
       <c r="E8" t="n">
-        <v>-1242239973</v>
+        <v>1242239973</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -710,7 +710,7 @@
         <v>111000000</v>
       </c>
       <c r="E9" t="n">
-        <v>-1006726625</v>
+        <v>1006726625</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         <v>98900000</v>
       </c>
       <c r="E11" t="n">
-        <v>-129241434</v>
+        <v>129241434</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -934,7 +934,7 @@
         <v>86900000</v>
       </c>
       <c r="E16" t="n">
-        <v>-1651573196</v>
+        <v>1651573196</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -966,7 +966,7 @@
         <v>83000000</v>
       </c>
       <c r="E17" t="n">
-        <v>-2079215104</v>
+        <v>2079215104</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1030,7 +1030,7 @@
         <v>75600000</v>
       </c>
       <c r="E19" t="n">
-        <v>-647842523</v>
+        <v>647842523</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1126,7 +1126,7 @@
         <v>71300000</v>
       </c>
       <c r="E22" t="n">
-        <v>-1430204134</v>
+        <v>1430204134</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
         <v>66500000</v>
       </c>
       <c r="E25" t="n">
-        <v>-1879119739</v>
+        <v>1879119739</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1254,7 +1254,7 @@
         <v>65900000</v>
       </c>
       <c r="E26" t="n">
-        <v>-1486790027</v>
+        <v>1486790027</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1286,7 +1286,7 @@
         <v>65600000</v>
       </c>
       <c r="E27" t="n">
-        <v>-1416746633</v>
+        <v>1416746633</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
         <v>61000000</v>
       </c>
       <c r="E29" t="n">
-        <v>-531540744</v>
+        <v>531540744</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
         <v>59500000</v>
       </c>
       <c r="E30" t="n">
-        <v>-938320026</v>
+        <v>938320026</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1414,7 +1414,7 @@
         <v>59500000</v>
       </c>
       <c r="E31" t="n">
-        <v>-813069390</v>
+        <v>813069390</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>59300000</v>
       </c>
       <c r="E32" t="n">
-        <v>-927935670</v>
+        <v>927935670</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1542,7 +1542,7 @@
         <v>57600000</v>
       </c>
       <c r="E35" t="n">
-        <v>-462050242</v>
+        <v>462050242</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
         <v>57200000</v>
       </c>
       <c r="E36" t="n">
-        <v>-1227626556</v>
+        <v>1227626556</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1702,7 +1702,7 @@
         <v>54000000</v>
       </c>
       <c r="E40" t="n">
-        <v>-2047307129</v>
+        <v>2047307129</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1798,7 +1798,7 @@
         <v>52900000</v>
       </c>
       <c r="E43" t="n">
-        <v>-180113786</v>
+        <v>180113786</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1830,7 +1830,7 @@
         <v>52700000</v>
       </c>
       <c r="E44" t="n">
-        <v>-1764961168</v>
+        <v>1764961168</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2022,7 +2022,7 @@
         <v>46800000</v>
       </c>
       <c r="E50" t="n">
-        <v>-2076790778</v>
+        <v>2076790778</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2182,7 +2182,7 @@
         <v>45500000</v>
       </c>
       <c r="E55" t="n">
-        <v>-86111251</v>
+        <v>86111251</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2214,7 +2214,7 @@
         <v>45200000</v>
       </c>
       <c r="E56" t="n">
-        <v>-577670911</v>
+        <v>577670911</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2246,7 +2246,7 @@
         <v>44700000</v>
       </c>
       <c r="E57" t="n">
-        <v>-761323764</v>
+        <v>761323764</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>44600000</v>
       </c>
       <c r="E58" t="n">
-        <v>-1810622589</v>
+        <v>1810622589</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2342,7 +2342,7 @@
         <v>44200000</v>
       </c>
       <c r="E60" t="n">
-        <v>-310851754</v>
+        <v>310851754</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
         <v>44200000</v>
       </c>
       <c r="E61" t="n">
-        <v>-20258086</v>
+        <v>20258086</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2406,7 +2406,7 @@
         <v>44200000</v>
       </c>
       <c r="E62" t="n">
-        <v>-1247067160</v>
+        <v>1247067160</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2438,7 +2438,7 @@
         <v>43700000</v>
       </c>
       <c r="E63" t="n">
-        <v>-637110</v>
+        <v>637110</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2566,7 +2566,7 @@
         <v>43200000</v>
       </c>
       <c r="E67" t="n">
-        <v>-714924979</v>
+        <v>714924979</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
@@ -2630,7 +2630,7 @@
         <v>42400000</v>
       </c>
       <c r="E69" t="n">
-        <v>-1250780788</v>
+        <v>1250780788</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
@@ -2662,7 +2662,7 @@
         <v>42400000</v>
       </c>
       <c r="E70" t="n">
-        <v>-1927140290</v>
+        <v>1927140290</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -2854,7 +2854,7 @@
         <v>40400000</v>
       </c>
       <c r="E76" t="n">
-        <v>-1179397924</v>
+        <v>1179397924</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -2886,7 +2886,7 @@
         <v>40300000</v>
       </c>
       <c r="E77" t="n">
-        <v>-239587100</v>
+        <v>239587100</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -2918,7 +2918,7 @@
         <v>39700000</v>
       </c>
       <c r="E78" t="n">
-        <v>-1884979616</v>
+        <v>1884979616</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -2982,7 +2982,7 @@
         <v>39200000</v>
       </c>
       <c r="E80" t="n">
-        <v>-1000954155</v>
+        <v>1000954155</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -3078,7 +3078,7 @@
         <v>39100000</v>
       </c>
       <c r="E83" t="n">
-        <v>-1061687511</v>
+        <v>1061687511</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -3142,7 +3142,7 @@
         <v>38900000</v>
       </c>
       <c r="E85" t="n">
-        <v>-615571470</v>
+        <v>615571470</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
         <v>38600000</v>
       </c>
       <c r="E86" t="n">
-        <v>-1250601472</v>
+        <v>1250601472</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -3238,7 +3238,7 @@
         <v>38300000</v>
       </c>
       <c r="E88" t="n">
-        <v>-461676798</v>
+        <v>461676798</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
@@ -3334,7 +3334,7 @@
         <v>38200000</v>
       </c>
       <c r="E91" t="n">
-        <v>-1545431583</v>
+        <v>1545431583</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
@@ -3494,7 +3494,7 @@
         <v>37200000</v>
       </c>
       <c r="E96" t="n">
-        <v>-777802467</v>
+        <v>777802467</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -3558,7 +3558,7 @@
         <v>37000000</v>
       </c>
       <c r="E98" t="n">
-        <v>-1580941859</v>
+        <v>1580941859</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -3590,7 +3590,7 @@
         <v>36700000</v>
       </c>
       <c r="E99" t="n">
-        <v>-2096681055</v>
+        <v>2096681055</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -3654,7 +3654,7 @@
         <v>36600000</v>
       </c>
       <c r="E101" t="n">
-        <v>-1526082738</v>
+        <v>1526082738</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -3718,7 +3718,7 @@
         <v>36300000</v>
       </c>
       <c r="E103" t="n">
-        <v>-1284182361</v>
+        <v>1284182361</v>
       </c>
       <c r="F103" t="inlineStr">
         <is>
@@ -3878,7 +3878,7 @@
         <v>35500000</v>
       </c>
       <c r="E108" t="n">
-        <v>-1522195762</v>
+        <v>1522195762</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -3910,7 +3910,7 @@
         <v>35500000</v>
       </c>
       <c r="E109" t="n">
-        <v>-1074845435</v>
+        <v>1074845435</v>
       </c>
       <c r="F109" t="inlineStr">
         <is>
@@ -4006,7 +4006,7 @@
         <v>35200000</v>
       </c>
       <c r="E112" t="n">
-        <v>-1176905261</v>
+        <v>1176905261</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -4038,7 +4038,7 @@
         <v>35200000</v>
       </c>
       <c r="E113" t="n">
-        <v>-534734650</v>
+        <v>534734650</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -4070,7 +4070,7 @@
         <v>34900000</v>
       </c>
       <c r="E114" t="n">
-        <v>-162406468</v>
+        <v>162406468</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -4102,7 +4102,7 @@
         <v>34600000</v>
       </c>
       <c r="E115" t="n">
-        <v>-168521051</v>
+        <v>168521051</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -4166,7 +4166,7 @@
         <v>34300000</v>
       </c>
       <c r="E117" t="n">
-        <v>-138366066</v>
+        <v>138366066</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -4230,7 +4230,7 @@
         <v>34000000</v>
       </c>
       <c r="E119" t="n">
-        <v>-331959881</v>
+        <v>331959881</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -4262,7 +4262,7 @@
         <v>34000000</v>
       </c>
       <c r="E120" t="n">
-        <v>-1533886064</v>
+        <v>1533886064</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -4294,7 +4294,7 @@
         <v>33800000</v>
       </c>
       <c r="E121" t="n">
-        <v>-1746939980</v>
+        <v>1746939980</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -4486,7 +4486,7 @@
         <v>33500000</v>
       </c>
       <c r="E127" t="n">
-        <v>-452856577</v>
+        <v>452856577</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
@@ -4518,7 +4518,7 @@
         <v>33500000</v>
       </c>
       <c r="E128" t="n">
-        <v>-1479092184</v>
+        <v>1479092184</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -4582,7 +4582,7 @@
         <v>33400000</v>
       </c>
       <c r="E130" t="n">
-        <v>-1204978913</v>
+        <v>1204978913</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -4742,7 +4742,7 @@
         <v>32700000</v>
       </c>
       <c r="E135" t="n">
-        <v>-1548520443</v>
+        <v>1548520443</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
@@ -4806,7 +4806,7 @@
         <v>32200000</v>
       </c>
       <c r="E137" t="n">
-        <v>-566427705</v>
+        <v>566427705</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -4998,7 +4998,7 @@
         <v>31900000</v>
       </c>
       <c r="E143" t="n">
-        <v>-2046528019</v>
+        <v>2046528019</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -5030,7 +5030,7 @@
         <v>31800000</v>
       </c>
       <c r="E144" t="n">
-        <v>-1827509902</v>
+        <v>1827509902</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -5094,7 +5094,7 @@
         <v>31700000</v>
       </c>
       <c r="E146" t="n">
-        <v>-702890308</v>
+        <v>702890308</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -5126,7 +5126,7 @@
         <v>31700000</v>
       </c>
       <c r="E147" t="n">
-        <v>-443090949</v>
+        <v>443090949</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -5158,7 +5158,7 @@
         <v>31700000</v>
       </c>
       <c r="E148" t="n">
-        <v>-1364951915</v>
+        <v>1364951915</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -5190,7 +5190,7 @@
         <v>31600000</v>
       </c>
       <c r="E149" t="n">
-        <v>-1269053597</v>
+        <v>1269053597</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -5254,7 +5254,7 @@
         <v>31400000</v>
       </c>
       <c r="E151" t="n">
-        <v>-2003106705</v>
+        <v>2003106705</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -5350,7 +5350,7 @@
         <v>31200000</v>
       </c>
       <c r="E154" t="n">
-        <v>-68143024</v>
+        <v>68143024</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -5414,7 +5414,7 @@
         <v>30700000</v>
       </c>
       <c r="E156" t="n">
-        <v>-386796822</v>
+        <v>386796822</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -5446,7 +5446,7 @@
         <v>30700000</v>
       </c>
       <c r="E157" t="n">
-        <v>-528909422</v>
+        <v>528909422</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -5478,7 +5478,7 @@
         <v>30700000</v>
       </c>
       <c r="E158" t="n">
-        <v>-1149805662</v>
+        <v>1149805662</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -5510,7 +5510,7 @@
         <v>30500000</v>
       </c>
       <c r="E159" t="n">
-        <v>-470011361</v>
+        <v>470011361</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -5734,7 +5734,7 @@
         <v>30200000</v>
       </c>
       <c r="E166" t="n">
-        <v>-1980539018</v>
+        <v>1980539018</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
@@ -5798,7 +5798,7 @@
         <v>30100000</v>
       </c>
       <c r="E168" t="n">
-        <v>-1312440652</v>
+        <v>1312440652</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
@@ -5830,7 +5830,7 @@
         <v>30100000</v>
       </c>
       <c r="E169" t="n">
-        <v>-1867827315</v>
+        <v>1867827315</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
@@ -5894,7 +5894,7 @@
         <v>30100000</v>
       </c>
       <c r="E171" t="n">
-        <v>-933243348</v>
+        <v>933243348</v>
       </c>
       <c r="F171" t="inlineStr">
         <is>
@@ -5926,7 +5926,7 @@
         <v>30000000</v>
       </c>
       <c r="E172" t="n">
-        <v>-53701033</v>
+        <v>53701033</v>
       </c>
       <c r="F172" t="inlineStr">
         <is>
@@ -6054,7 +6054,7 @@
         <v>29300000</v>
       </c>
       <c r="E176" t="n">
-        <v>-247891344</v>
+        <v>247891344</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -6118,7 +6118,7 @@
         <v>29200000</v>
       </c>
       <c r="E178" t="n">
-        <v>-1257464041</v>
+        <v>1257464041</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
@@ -6150,7 +6150,7 @@
         <v>29200000</v>
       </c>
       <c r="E179" t="n">
-        <v>-215825623</v>
+        <v>215825623</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
@@ -6182,7 +6182,7 @@
         <v>29000000</v>
       </c>
       <c r="E180" t="n">
-        <v>-2008598415</v>
+        <v>2008598415</v>
       </c>
       <c r="F180" t="inlineStr">
         <is>
@@ -6406,7 +6406,7 @@
         <v>28300000</v>
       </c>
       <c r="E187" t="n">
-        <v>-1924866811</v>
+        <v>1924866811</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
@@ -6438,7 +6438,7 @@
         <v>28200000</v>
       </c>
       <c r="E188" t="n">
-        <v>-989193599</v>
+        <v>989193599</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -6502,7 +6502,7 @@
         <v>28100000</v>
       </c>
       <c r="E190" t="n">
-        <v>-1860974066</v>
+        <v>1860974066</v>
       </c>
       <c r="F190" t="inlineStr">
         <is>
@@ -6566,7 +6566,7 @@
         <v>27800000</v>
       </c>
       <c r="E192" t="n">
-        <v>-1991898075</v>
+        <v>1991898075</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -6598,7 +6598,7 @@
         <v>27800000</v>
       </c>
       <c r="E193" t="n">
-        <v>-436985012</v>
+        <v>436985012</v>
       </c>
       <c r="F193" t="inlineStr">
         <is>
@@ -6630,7 +6630,7 @@
         <v>27700000</v>
       </c>
       <c r="E194" t="n">
-        <v>-1402186668</v>
+        <v>1402186668</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -6726,7 +6726,7 @@
         <v>27400000</v>
       </c>
       <c r="E197" t="n">
-        <v>-1591686463</v>
+        <v>1591686463</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
@@ -6790,7 +6790,7 @@
         <v>27400000</v>
       </c>
       <c r="E199" t="n">
-        <v>-2056948970</v>
+        <v>2056948970</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -6854,7 +6854,7 @@
         <v>27300000</v>
       </c>
       <c r="E201" t="n">
-        <v>-884442242</v>
+        <v>884442242</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -6886,7 +6886,7 @@
         <v>27100000</v>
       </c>
       <c r="E202" t="n">
-        <v>-1262986956</v>
+        <v>1262986956</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -6950,7 +6950,7 @@
         <v>27100000</v>
       </c>
       <c r="E204" t="n">
-        <v>-152457007</v>
+        <v>152457007</v>
       </c>
       <c r="F204" t="inlineStr">
         <is>
@@ -6982,7 +6982,7 @@
         <v>27000000</v>
       </c>
       <c r="E205" t="n">
-        <v>-2018998613</v>
+        <v>2018998613</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -7014,7 +7014,7 @@
         <v>26900000</v>
       </c>
       <c r="E206" t="n">
-        <v>-651317951</v>
+        <v>651317951</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -7110,7 +7110,7 @@
         <v>26700000</v>
       </c>
       <c r="E209" t="n">
-        <v>-1416265687</v>
+        <v>1416265687</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -7142,7 +7142,7 @@
         <v>26500000</v>
       </c>
       <c r="E210" t="n">
-        <v>-2114115729</v>
+        <v>2114115729</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -7174,7 +7174,7 @@
         <v>26500000</v>
       </c>
       <c r="E211" t="n">
-        <v>-1116719150</v>
+        <v>1116719150</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -7366,7 +7366,7 @@
         <v>26200000</v>
       </c>
       <c r="E217" t="n">
-        <v>-1082338097</v>
+        <v>1082338097</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>
@@ -7430,7 +7430,7 @@
         <v>26100000</v>
       </c>
       <c r="E219" t="n">
-        <v>-703494393</v>
+        <v>703494393</v>
       </c>
       <c r="F219" t="inlineStr">
         <is>
@@ -7558,7 +7558,7 @@
         <v>25900000</v>
       </c>
       <c r="E223" t="n">
-        <v>-1512829999</v>
+        <v>1512829999</v>
       </c>
       <c r="F223" t="inlineStr">
         <is>
@@ -7590,7 +7590,7 @@
         <v>25800000</v>
       </c>
       <c r="E224" t="n">
-        <v>-1638447346</v>
+        <v>1638447346</v>
       </c>
       <c r="F224" t="inlineStr">
         <is>
@@ -7654,7 +7654,7 @@
         <v>25700000</v>
       </c>
       <c r="E226" t="n">
-        <v>-1123008332</v>
+        <v>1123008332</v>
       </c>
       <c r="F226" t="inlineStr">
         <is>
@@ -7718,7 +7718,7 @@
         <v>25600000</v>
       </c>
       <c r="E228" t="n">
-        <v>-627208632</v>
+        <v>627208632</v>
       </c>
       <c r="F228" t="inlineStr">
         <is>
@@ -7750,7 +7750,7 @@
         <v>25600000</v>
       </c>
       <c r="E229" t="n">
-        <v>-177425484</v>
+        <v>177425484</v>
       </c>
       <c r="F229" t="inlineStr">
         <is>
@@ -7782,7 +7782,7 @@
         <v>25500000</v>
       </c>
       <c r="E230" t="n">
-        <v>-1568050209</v>
+        <v>1568050209</v>
       </c>
       <c r="F230" t="inlineStr">
         <is>
@@ -7878,7 +7878,7 @@
         <v>25400000</v>
       </c>
       <c r="E233" t="n">
-        <v>-59256302</v>
+        <v>59256302</v>
       </c>
       <c r="F233" t="inlineStr">
         <is>
@@ -7974,7 +7974,7 @@
         <v>25200000</v>
       </c>
       <c r="E236" t="n">
-        <v>-1803299520</v>
+        <v>1803299520</v>
       </c>
       <c r="F236" t="inlineStr">
         <is>
@@ -8006,7 +8006,7 @@
         <v>25200000</v>
       </c>
       <c r="E237" t="n">
-        <v>-621571211</v>
+        <v>621571211</v>
       </c>
       <c r="F237" t="inlineStr">
         <is>
@@ -8038,7 +8038,7 @@
         <v>25200000</v>
       </c>
       <c r="E238" t="n">
-        <v>-1659299688</v>
+        <v>1659299688</v>
       </c>
       <c r="F238" t="inlineStr">
         <is>
@@ -8102,7 +8102,7 @@
         <v>25100000</v>
       </c>
       <c r="E240" t="n">
-        <v>-2016028772</v>
+        <v>2016028772</v>
       </c>
       <c r="F240" t="inlineStr">
         <is>
@@ -8134,7 +8134,7 @@
         <v>25100000</v>
       </c>
       <c r="E241" t="n">
-        <v>-822804986</v>
+        <v>822804986</v>
       </c>
       <c r="F241" t="inlineStr">
         <is>
@@ -8262,7 +8262,7 @@
         <v>24800000</v>
       </c>
       <c r="E245" t="n">
-        <v>-1706466181</v>
+        <v>1706466181</v>
       </c>
       <c r="F245" t="inlineStr">
         <is>
@@ -8294,7 +8294,7 @@
         <v>24800000</v>
       </c>
       <c r="E246" t="n">
-        <v>-595614592</v>
+        <v>595614592</v>
       </c>
       <c r="F246" t="inlineStr">
         <is>
@@ -8358,7 +8358,7 @@
         <v>24700000</v>
       </c>
       <c r="E248" t="n">
-        <v>-943131953</v>
+        <v>943131953</v>
       </c>
       <c r="F248" t="inlineStr">
         <is>
@@ -8390,7 +8390,7 @@
         <v>24700000</v>
       </c>
       <c r="E249" t="n">
-        <v>-1300240884</v>
+        <v>1300240884</v>
       </c>
       <c r="F249" t="inlineStr">
         <is>
@@ -8422,7 +8422,7 @@
         <v>24600000</v>
       </c>
       <c r="E250" t="n">
-        <v>-2014011234</v>
+        <v>2014011234</v>
       </c>
       <c r="F250" t="inlineStr">
         <is>
@@ -8454,7 +8454,7 @@
         <v>24600000</v>
       </c>
       <c r="E251" t="n">
-        <v>-646979997</v>
+        <v>646979997</v>
       </c>
       <c r="F251" t="inlineStr">
         <is>
@@ -8486,7 +8486,7 @@
         <v>24500000</v>
       </c>
       <c r="E252" t="n">
-        <v>-1807732832</v>
+        <v>1807732832</v>
       </c>
       <c r="F252" t="inlineStr">
         <is>
@@ -8518,7 +8518,7 @@
         <v>24400000</v>
       </c>
       <c r="E253" t="n">
-        <v>-498976893</v>
+        <v>498976893</v>
       </c>
       <c r="F253" t="inlineStr">
         <is>
@@ -8550,7 +8550,7 @@
         <v>24300000</v>
       </c>
       <c r="E254" t="n">
-        <v>-1914718397</v>
+        <v>1914718397</v>
       </c>
       <c r="F254" t="inlineStr">
         <is>
@@ -8582,7 +8582,7 @@
         <v>24300000</v>
       </c>
       <c r="E255" t="n">
-        <v>-1981161397</v>
+        <v>1981161397</v>
       </c>
       <c r="F255" t="inlineStr">
         <is>
@@ -8614,7 +8614,7 @@
         <v>24200000</v>
       </c>
       <c r="E256" t="n">
-        <v>-1594053126</v>
+        <v>1594053126</v>
       </c>
       <c r="F256" t="inlineStr">
         <is>
@@ -8646,7 +8646,7 @@
         <v>24200000</v>
       </c>
       <c r="E257" t="n">
-        <v>-1455709001</v>
+        <v>1455709001</v>
       </c>
       <c r="F257" t="inlineStr">
         <is>
@@ -8710,7 +8710,7 @@
         <v>24100000</v>
       </c>
       <c r="E259" t="n">
-        <v>-1885901409</v>
+        <v>1885901409</v>
       </c>
       <c r="F259" t="inlineStr">
         <is>
@@ -8806,7 +8806,7 @@
         <v>24100000</v>
       </c>
       <c r="E262" t="n">
-        <v>-164428673</v>
+        <v>164428673</v>
       </c>
       <c r="F262" t="inlineStr">
         <is>
@@ -8838,7 +8838,7 @@
         <v>24100000</v>
       </c>
       <c r="E263" t="n">
-        <v>-1843640592</v>
+        <v>1843640592</v>
       </c>
       <c r="F263" t="inlineStr">
         <is>
@@ -8966,7 +8966,7 @@
         <v>24000000</v>
       </c>
       <c r="E267" t="n">
-        <v>-310930150</v>
+        <v>310930150</v>
       </c>
       <c r="F267" t="inlineStr">
         <is>
@@ -8998,7 +8998,7 @@
         <v>23900000</v>
       </c>
       <c r="E268" t="n">
-        <v>-227088365</v>
+        <v>227088365</v>
       </c>
       <c r="F268" t="inlineStr">
         <is>
@@ -9030,7 +9030,7 @@
         <v>23900000</v>
       </c>
       <c r="E269" t="n">
-        <v>-2007001967</v>
+        <v>2007001967</v>
       </c>
       <c r="F269" t="inlineStr">
         <is>
@@ -9062,7 +9062,7 @@
         <v>23900000</v>
       </c>
       <c r="E270" t="n">
-        <v>-1376435507</v>
+        <v>1376435507</v>
       </c>
       <c r="F270" t="inlineStr">
         <is>
@@ -9190,7 +9190,7 @@
         <v>23700000</v>
       </c>
       <c r="E274" t="n">
-        <v>-1751157342</v>
+        <v>1751157342</v>
       </c>
       <c r="F274" t="inlineStr">
         <is>
@@ -9222,7 +9222,7 @@
         <v>23700000</v>
       </c>
       <c r="E275" t="n">
-        <v>-1138142460</v>
+        <v>1138142460</v>
       </c>
       <c r="F275" t="inlineStr">
         <is>
@@ -9254,7 +9254,7 @@
         <v>23700000</v>
       </c>
       <c r="E276" t="n">
-        <v>-1669715381</v>
+        <v>1669715381</v>
       </c>
       <c r="F276" t="inlineStr">
         <is>
@@ -9286,7 +9286,7 @@
         <v>23700000</v>
       </c>
       <c r="E277" t="n">
-        <v>-1185147091</v>
+        <v>1185147091</v>
       </c>
       <c r="F277" t="inlineStr">
         <is>
@@ -9318,7 +9318,7 @@
         <v>23600000</v>
       </c>
       <c r="E278" t="n">
-        <v>-1278044343</v>
+        <v>1278044343</v>
       </c>
       <c r="F278" t="inlineStr">
         <is>
@@ -9414,7 +9414,7 @@
         <v>23600000</v>
       </c>
       <c r="E281" t="n">
-        <v>-1823473522</v>
+        <v>1823473522</v>
       </c>
       <c r="F281" t="inlineStr">
         <is>
@@ -9446,7 +9446,7 @@
         <v>23600000</v>
       </c>
       <c r="E282" t="n">
-        <v>-669297392</v>
+        <v>669297392</v>
       </c>
       <c r="F282" t="inlineStr">
         <is>
@@ -9574,7 +9574,7 @@
         <v>23400000</v>
       </c>
       <c r="E286" t="n">
-        <v>-663035456</v>
+        <v>663035456</v>
       </c>
       <c r="F286" t="inlineStr">
         <is>
@@ -9670,7 +9670,7 @@
         <v>23200000</v>
       </c>
       <c r="E289" t="n">
-        <v>-1428207971</v>
+        <v>1428207971</v>
       </c>
       <c r="F289" t="inlineStr">
         <is>
@@ -9702,7 +9702,7 @@
         <v>23200000</v>
       </c>
       <c r="E290" t="n">
-        <v>-623214445</v>
+        <v>623214445</v>
       </c>
       <c r="F290" t="inlineStr">
         <is>
@@ -9766,7 +9766,7 @@
         <v>23100000</v>
       </c>
       <c r="E292" t="n">
-        <v>-189972695</v>
+        <v>189972695</v>
       </c>
       <c r="F292" t="inlineStr">
         <is>
@@ -9798,7 +9798,7 @@
         <v>23100000</v>
       </c>
       <c r="E293" t="n">
-        <v>-1743853874</v>
+        <v>1743853874</v>
       </c>
       <c r="F293" t="inlineStr">
         <is>
@@ -9926,7 +9926,7 @@
         <v>23000000</v>
       </c>
       <c r="E297" t="n">
-        <v>-916919913</v>
+        <v>916919913</v>
       </c>
       <c r="F297" t="inlineStr">
         <is>
@@ -9990,7 +9990,7 @@
         <v>23000000</v>
       </c>
       <c r="E299" t="n">
-        <v>-1944935404</v>
+        <v>1944935404</v>
       </c>
       <c r="F299" t="inlineStr">
         <is>
@@ -10086,7 +10086,7 @@
         <v>22900000</v>
       </c>
       <c r="E302" t="n">
-        <v>-881526355</v>
+        <v>881526355</v>
       </c>
       <c r="F302" t="inlineStr">
         <is>
@@ -10214,7 +10214,7 @@
         <v>22700000</v>
       </c>
       <c r="E306" t="n">
-        <v>-1316783767</v>
+        <v>1316783767</v>
       </c>
       <c r="F306" t="inlineStr">
         <is>
@@ -10246,7 +10246,7 @@
         <v>22600000</v>
       </c>
       <c r="E307" t="n">
-        <v>-627798328</v>
+        <v>627798328</v>
       </c>
       <c r="F307" t="inlineStr">
         <is>
@@ -10438,7 +10438,7 @@
         <v>22500000</v>
       </c>
       <c r="E313" t="n">
-        <v>-1863812858</v>
+        <v>1863812858</v>
       </c>
       <c r="F313" t="inlineStr">
         <is>
@@ -10534,7 +10534,7 @@
         <v>22400000</v>
       </c>
       <c r="E316" t="n">
-        <v>-549898383</v>
+        <v>549898383</v>
       </c>
       <c r="F316" t="inlineStr">
         <is>
@@ -10598,7 +10598,7 @@
         <v>22300000</v>
       </c>
       <c r="E318" t="n">
-        <v>-1710466919</v>
+        <v>1710466919</v>
       </c>
       <c r="F318" t="inlineStr">
         <is>
@@ -10630,7 +10630,7 @@
         <v>22200000</v>
       </c>
       <c r="E319" t="n">
-        <v>-1748635427</v>
+        <v>1748635427</v>
       </c>
       <c r="F319" t="inlineStr">
         <is>
@@ -10822,7 +10822,7 @@
         <v>21900000</v>
       </c>
       <c r="E325" t="n">
-        <v>-1627798338</v>
+        <v>1627798338</v>
       </c>
       <c r="F325" t="inlineStr">
         <is>
@@ -10854,7 +10854,7 @@
         <v>21900000</v>
       </c>
       <c r="E326" t="n">
-        <v>-817264729</v>
+        <v>817264729</v>
       </c>
       <c r="F326" t="inlineStr">
         <is>
@@ -10950,7 +10950,7 @@
         <v>21800000</v>
       </c>
       <c r="E329" t="n">
-        <v>-1596542523</v>
+        <v>1596542523</v>
       </c>
       <c r="F329" t="inlineStr">
         <is>
@@ -10982,7 +10982,7 @@
         <v>21800000</v>
       </c>
       <c r="E330" t="n">
-        <v>-744669884</v>
+        <v>744669884</v>
       </c>
       <c r="F330" t="inlineStr">
         <is>
@@ -11014,7 +11014,7 @@
         <v>21800000</v>
       </c>
       <c r="E331" t="n">
-        <v>-2145485337</v>
+        <v>2145485337</v>
       </c>
       <c r="F331" t="inlineStr">
         <is>
@@ -11046,7 +11046,7 @@
         <v>21800000</v>
       </c>
       <c r="E332" t="n">
-        <v>-809000405</v>
+        <v>809000405</v>
       </c>
       <c r="F332" t="inlineStr">
         <is>
@@ -11110,7 +11110,7 @@
         <v>21700000</v>
       </c>
       <c r="E334" t="n">
-        <v>-82115715</v>
+        <v>82115715</v>
       </c>
       <c r="F334" t="inlineStr">
         <is>
@@ -11334,7 +11334,7 @@
         <v>21500000</v>
       </c>
       <c r="E341" t="n">
-        <v>-180292870</v>
+        <v>180292870</v>
       </c>
       <c r="F341" t="inlineStr">
         <is>
@@ -11494,7 +11494,7 @@
         <v>21300000</v>
       </c>
       <c r="E346" t="n">
-        <v>-123648049</v>
+        <v>123648049</v>
       </c>
       <c r="F346" t="inlineStr">
         <is>
@@ -11654,7 +11654,7 @@
         <v>21200000</v>
       </c>
       <c r="E351" t="n">
-        <v>-1519993272</v>
+        <v>1519993272</v>
       </c>
       <c r="F351" t="inlineStr">
         <is>
@@ -11782,7 +11782,7 @@
         <v>21000000</v>
       </c>
       <c r="E355" t="n">
-        <v>-827028929</v>
+        <v>827028929</v>
       </c>
       <c r="F355" t="inlineStr">
         <is>
@@ -11910,7 +11910,7 @@
         <v>20900000</v>
       </c>
       <c r="E359" t="n">
-        <v>-466966709</v>
+        <v>466966709</v>
       </c>
       <c r="F359" t="inlineStr">
         <is>
@@ -11974,7 +11974,7 @@
         <v>20900000</v>
       </c>
       <c r="E361" t="n">
-        <v>-1826852003</v>
+        <v>1826852003</v>
       </c>
       <c r="F361" t="inlineStr">
         <is>
@@ -12102,7 +12102,7 @@
         <v>20800000</v>
       </c>
       <c r="E365" t="n">
-        <v>-1916519167</v>
+        <v>1916519167</v>
       </c>
       <c r="F365" t="inlineStr">
         <is>
@@ -12262,7 +12262,7 @@
         <v>20700000</v>
       </c>
       <c r="E370" t="n">
-        <v>-260022156</v>
+        <v>260022156</v>
       </c>
       <c r="F370" t="inlineStr">
         <is>
@@ -12326,7 +12326,7 @@
         <v>20600000</v>
       </c>
       <c r="E372" t="n">
-        <v>-932762612</v>
+        <v>932762612</v>
       </c>
       <c r="F372" t="inlineStr">
         <is>
@@ -12390,7 +12390,7 @@
         <v>20500000</v>
       </c>
       <c r="E374" t="n">
-        <v>-2141275301</v>
+        <v>2141275301</v>
       </c>
       <c r="F374" t="inlineStr">
         <is>
@@ -12454,7 +12454,7 @@
         <v>20500000</v>
       </c>
       <c r="E376" t="n">
-        <v>-1875753309</v>
+        <v>1875753309</v>
       </c>
       <c r="F376" t="inlineStr">
         <is>
@@ -12518,7 +12518,7 @@
         <v>20400000</v>
       </c>
       <c r="E378" t="n">
-        <v>-1278612224</v>
+        <v>1278612224</v>
       </c>
       <c r="F378" t="inlineStr">
         <is>
@@ -12582,7 +12582,7 @@
         <v>20400000</v>
       </c>
       <c r="E380" t="n">
-        <v>-658564452</v>
+        <v>658564452</v>
       </c>
       <c r="F380" t="inlineStr">
         <is>
@@ -12646,7 +12646,7 @@
         <v>20400000</v>
       </c>
       <c r="E382" t="n">
-        <v>-715412172</v>
+        <v>715412172</v>
       </c>
       <c r="F382" t="inlineStr">
         <is>
@@ -12678,7 +12678,7 @@
         <v>20300000</v>
       </c>
       <c r="E383" t="n">
-        <v>-1853678595</v>
+        <v>1853678595</v>
       </c>
       <c r="F383" t="inlineStr">
         <is>
@@ -12710,7 +12710,7 @@
         <v>20300000</v>
       </c>
       <c r="E384" t="n">
-        <v>-1862510549</v>
+        <v>1862510549</v>
       </c>
       <c r="F384" t="inlineStr">
         <is>
@@ -12742,7 +12742,7 @@
         <v>20300000</v>
       </c>
       <c r="E385" t="n">
-        <v>-1065850336</v>
+        <v>1065850336</v>
       </c>
       <c r="F385" t="inlineStr">
         <is>
@@ -12774,7 +12774,7 @@
         <v>20200000</v>
       </c>
       <c r="E386" t="n">
-        <v>-1343053096</v>
+        <v>1343053096</v>
       </c>
       <c r="F386" t="inlineStr">
         <is>
@@ -12806,7 +12806,7 @@
         <v>20200000</v>
       </c>
       <c r="E387" t="n">
-        <v>-1530839327</v>
+        <v>1530839327</v>
       </c>
       <c r="F387" t="inlineStr">
         <is>
@@ -12838,7 +12838,7 @@
         <v>20200000</v>
       </c>
       <c r="E388" t="n">
-        <v>-1523223269</v>
+        <v>1523223269</v>
       </c>
       <c r="F388" t="inlineStr">
         <is>
@@ -12870,7 +12870,7 @@
         <v>20200000</v>
       </c>
       <c r="E389" t="n">
-        <v>-1315784346</v>
+        <v>1315784346</v>
       </c>
       <c r="F389" t="inlineStr">
         <is>
@@ -12902,7 +12902,7 @@
         <v>20200000</v>
       </c>
       <c r="E390" t="n">
-        <v>-555432760</v>
+        <v>555432760</v>
       </c>
       <c r="F390" t="inlineStr">
         <is>
@@ -12934,7 +12934,7 @@
         <v>20200000</v>
       </c>
       <c r="E391" t="n">
-        <v>-1780571122</v>
+        <v>1780571122</v>
       </c>
       <c r="F391" t="inlineStr">
         <is>
@@ -13030,7 +13030,7 @@
         <v>20100000</v>
       </c>
       <c r="E394" t="n">
-        <v>-1971410434</v>
+        <v>1971410434</v>
       </c>
       <c r="F394" t="inlineStr">
         <is>
@@ -13126,7 +13126,7 @@
         <v>20100000</v>
       </c>
       <c r="E397" t="n">
-        <v>-1567591953</v>
+        <v>1567591953</v>
       </c>
       <c r="F397" t="inlineStr">
         <is>
@@ -13350,7 +13350,7 @@
         <v>20000000</v>
       </c>
       <c r="E404" t="n">
-        <v>-419795061</v>
+        <v>419795061</v>
       </c>
       <c r="F404" t="inlineStr">
         <is>
@@ -13478,7 +13478,7 @@
         <v>19800000</v>
       </c>
       <c r="E408" t="n">
-        <v>-1060087212</v>
+        <v>1060087212</v>
       </c>
       <c r="F408" t="inlineStr">
         <is>
@@ -13542,7 +13542,7 @@
         <v>19800000</v>
       </c>
       <c r="E410" t="n">
-        <v>-591421943</v>
+        <v>591421943</v>
       </c>
       <c r="F410" t="inlineStr">
         <is>
@@ -13606,7 +13606,7 @@
         <v>19700000</v>
       </c>
       <c r="E412" t="n">
-        <v>-1137266977</v>
+        <v>1137266977</v>
       </c>
       <c r="F412" t="inlineStr">
         <is>
@@ -13638,7 +13638,7 @@
         <v>19700000</v>
       </c>
       <c r="E413" t="n">
-        <v>-1929282073</v>
+        <v>1929282073</v>
       </c>
       <c r="F413" t="inlineStr">
         <is>
@@ -13670,7 +13670,7 @@
         <v>19700000</v>
       </c>
       <c r="E414" t="n">
-        <v>-1561284392</v>
+        <v>1561284392</v>
       </c>
       <c r="F414" t="inlineStr">
         <is>
@@ -13734,7 +13734,7 @@
         <v>19600000</v>
       </c>
       <c r="E416" t="n">
-        <v>-1443942866</v>
+        <v>1443942866</v>
       </c>
       <c r="F416" t="inlineStr">
         <is>
@@ -13830,7 +13830,7 @@
         <v>19600000</v>
       </c>
       <c r="E419" t="n">
-        <v>-683752816</v>
+        <v>683752816</v>
       </c>
       <c r="F419" t="inlineStr">
         <is>
@@ -13862,7 +13862,7 @@
         <v>19600000</v>
       </c>
       <c r="E420" t="n">
-        <v>-333648858</v>
+        <v>333648858</v>
       </c>
       <c r="F420" t="inlineStr">
         <is>
@@ -13926,7 +13926,7 @@
         <v>19400000</v>
       </c>
       <c r="E422" t="n">
-        <v>-2039424704</v>
+        <v>2039424704</v>
       </c>
       <c r="F422" t="inlineStr">
         <is>
@@ -14086,7 +14086,7 @@
         <v>19300000</v>
       </c>
       <c r="E427" t="n">
-        <v>-1397060164</v>
+        <v>1397060164</v>
       </c>
       <c r="F427" t="inlineStr">
         <is>
@@ -14182,7 +14182,7 @@
         <v>19200000</v>
       </c>
       <c r="E430" t="n">
-        <v>-999352568</v>
+        <v>999352568</v>
       </c>
       <c r="F430" t="inlineStr">
         <is>
@@ -14374,7 +14374,7 @@
         <v>19000000</v>
       </c>
       <c r="E436" t="n">
-        <v>-1360759270</v>
+        <v>1360759270</v>
       </c>
       <c r="F436" t="inlineStr">
         <is>
@@ -14406,7 +14406,7 @@
         <v>19000000</v>
       </c>
       <c r="E437" t="n">
-        <v>-308210199</v>
+        <v>308210199</v>
       </c>
       <c r="F437" t="inlineStr">
         <is>
@@ -14470,7 +14470,7 @@
         <v>19000000</v>
       </c>
       <c r="E439" t="n">
-        <v>-1165824566</v>
+        <v>1165824566</v>
       </c>
       <c r="F439" t="inlineStr">
         <is>
@@ -14502,7 +14502,7 @@
         <v>19000000</v>
       </c>
       <c r="E440" t="n">
-        <v>-2053776676</v>
+        <v>2053776676</v>
       </c>
       <c r="F440" t="inlineStr">
         <is>
@@ -14534,7 +14534,7 @@
         <v>18900000</v>
       </c>
       <c r="E441" t="n">
-        <v>-1439448146</v>
+        <v>1439448146</v>
       </c>
       <c r="F441" t="inlineStr">
         <is>
@@ -14566,7 +14566,7 @@
         <v>18900000</v>
       </c>
       <c r="E442" t="n">
-        <v>-288203255</v>
+        <v>288203255</v>
       </c>
       <c r="F442" t="inlineStr">
         <is>
@@ -14630,7 +14630,7 @@
         <v>18800000</v>
       </c>
       <c r="E444" t="n">
-        <v>-640345728</v>
+        <v>640345728</v>
       </c>
       <c r="F444" t="inlineStr">
         <is>
@@ -14694,7 +14694,7 @@
         <v>18800000</v>
       </c>
       <c r="E446" t="n">
-        <v>-955504404</v>
+        <v>955504404</v>
       </c>
       <c r="F446" t="inlineStr">
         <is>
@@ -14726,7 +14726,7 @@
         <v>18800000</v>
       </c>
       <c r="E447" t="n">
-        <v>-827857580</v>
+        <v>827857580</v>
       </c>
       <c r="F447" t="inlineStr">
         <is>
@@ -14822,7 +14822,7 @@
         <v>18800000</v>
       </c>
       <c r="E450" t="n">
-        <v>-1018075758</v>
+        <v>1018075758</v>
       </c>
       <c r="F450" t="inlineStr">
         <is>
@@ -14854,7 +14854,7 @@
         <v>18700000</v>
       </c>
       <c r="E451" t="n">
-        <v>-589264726</v>
+        <v>589264726</v>
       </c>
       <c r="F451" t="inlineStr">
         <is>
@@ -14950,7 +14950,7 @@
         <v>18600000</v>
       </c>
       <c r="E454" t="n">
-        <v>-1581684096</v>
+        <v>1581684096</v>
       </c>
       <c r="F454" t="inlineStr">
         <is>
@@ -14982,7 +14982,7 @@
         <v>18600000</v>
       </c>
       <c r="E455" t="n">
-        <v>-1278132204</v>
+        <v>1278132204</v>
       </c>
       <c r="F455" t="inlineStr">
         <is>
@@ -15046,7 +15046,7 @@
         <v>18500000</v>
       </c>
       <c r="E457" t="n">
-        <v>-1386846400</v>
+        <v>1386846400</v>
       </c>
       <c r="F457" t="inlineStr">
         <is>
@@ -15078,7 +15078,7 @@
         <v>18500000</v>
       </c>
       <c r="E458" t="n">
-        <v>-837348935</v>
+        <v>837348935</v>
       </c>
       <c r="F458" t="inlineStr">
         <is>
@@ -15142,7 +15142,7 @@
         <v>18500000</v>
       </c>
       <c r="E460" t="n">
-        <v>-442358708</v>
+        <v>442358708</v>
       </c>
       <c r="F460" t="inlineStr">
         <is>
@@ -15174,7 +15174,7 @@
         <v>18500000</v>
       </c>
       <c r="E461" t="n">
-        <v>-243895108</v>
+        <v>243895108</v>
       </c>
       <c r="F461" t="inlineStr">
         <is>
@@ -15206,7 +15206,7 @@
         <v>18400000</v>
       </c>
       <c r="E462" t="n">
-        <v>-174642986</v>
+        <v>174642986</v>
       </c>
       <c r="F462" t="inlineStr">
         <is>
@@ -15238,7 +15238,7 @@
         <v>18400000</v>
       </c>
       <c r="E463" t="n">
-        <v>-1551107066</v>
+        <v>1551107066</v>
       </c>
       <c r="F463" t="inlineStr">
         <is>
@@ -15270,7 +15270,7 @@
         <v>18400000</v>
       </c>
       <c r="E464" t="n">
-        <v>-1340604095</v>
+        <v>1340604095</v>
       </c>
       <c r="F464" t="inlineStr">
         <is>
@@ -15302,7 +15302,7 @@
         <v>18400000</v>
       </c>
       <c r="E465" t="n">
-        <v>-1604169506</v>
+        <v>1604169506</v>
       </c>
       <c r="F465" t="inlineStr">
         <is>
@@ -15334,7 +15334,7 @@
         <v>18400000</v>
       </c>
       <c r="E466" t="n">
-        <v>-402677484</v>
+        <v>402677484</v>
       </c>
       <c r="F466" t="inlineStr">
         <is>
@@ -15398,7 +15398,7 @@
         <v>18300000</v>
       </c>
       <c r="E468" t="n">
-        <v>-829115004</v>
+        <v>829115004</v>
       </c>
       <c r="F468" t="inlineStr">
         <is>
@@ -15526,7 +15526,7 @@
         <v>18200000</v>
       </c>
       <c r="E472" t="n">
-        <v>-1081642841</v>
+        <v>1081642841</v>
       </c>
       <c r="F472" t="inlineStr">
         <is>
@@ -15590,7 +15590,7 @@
         <v>18100000</v>
       </c>
       <c r="E474" t="n">
-        <v>-988724622</v>
+        <v>988724622</v>
       </c>
       <c r="F474" t="inlineStr">
         <is>
@@ -15718,7 +15718,7 @@
         <v>18100000</v>
       </c>
       <c r="E478" t="n">
-        <v>-635073002</v>
+        <v>635073002</v>
       </c>
       <c r="F478" t="inlineStr">
         <is>
@@ -15750,7 +15750,7 @@
         <v>18000000</v>
       </c>
       <c r="E479" t="n">
-        <v>-313976048</v>
+        <v>313976048</v>
       </c>
       <c r="F479" t="inlineStr">
         <is>
@@ -15814,7 +15814,7 @@
         <v>18000000</v>
       </c>
       <c r="E481" t="n">
-        <v>-1767536179</v>
+        <v>1767536179</v>
       </c>
       <c r="F481" t="inlineStr">
         <is>
@@ -15974,7 +15974,7 @@
         <v>17900000</v>
       </c>
       <c r="E486" t="n">
-        <v>-1413362293</v>
+        <v>1413362293</v>
       </c>
       <c r="F486" t="inlineStr">
         <is>
@@ -16006,7 +16006,7 @@
         <v>17900000</v>
       </c>
       <c r="E487" t="n">
-        <v>-453761831</v>
+        <v>453761831</v>
       </c>
       <c r="F487" t="inlineStr">
         <is>
@@ -16102,7 +16102,7 @@
         <v>17900000</v>
       </c>
       <c r="E490" t="n">
-        <v>-1701859648</v>
+        <v>1701859648</v>
       </c>
       <c r="F490" t="inlineStr">
         <is>
@@ -16198,7 +16198,7 @@
         <v>17900000</v>
       </c>
       <c r="E493" t="n">
-        <v>-1005339138</v>
+        <v>1005339138</v>
       </c>
       <c r="F493" t="inlineStr">
         <is>
@@ -16230,7 +16230,7 @@
         <v>17900000</v>
       </c>
       <c r="E494" t="n">
-        <v>-1843665134</v>
+        <v>1843665134</v>
       </c>
       <c r="F494" t="inlineStr">
         <is>
@@ -16262,7 +16262,7 @@
         <v>17800000</v>
       </c>
       <c r="E495" t="n">
-        <v>-1826956705</v>
+        <v>1826956705</v>
       </c>
       <c r="F495" t="inlineStr">
         <is>
@@ -16294,7 +16294,7 @@
         <v>17800000</v>
       </c>
       <c r="E496" t="n">
-        <v>-1230053</v>
+        <v>1230053</v>
       </c>
       <c r="F496" t="inlineStr">
         <is>
@@ -16358,7 +16358,7 @@
         <v>17700000</v>
       </c>
       <c r="E498" t="n">
-        <v>-1202312948</v>
+        <v>1202312948</v>
       </c>
       <c r="F498" t="inlineStr">
         <is>
@@ -16390,7 +16390,7 @@
         <v>17700000</v>
       </c>
       <c r="E499" t="n">
-        <v>-1359291772</v>
+        <v>1359291772</v>
       </c>
       <c r="F499" t="inlineStr">
         <is>
@@ -16422,7 +16422,7 @@
         <v>17700000</v>
       </c>
       <c r="E500" t="n">
-        <v>-677201389</v>
+        <v>677201389</v>
       </c>
       <c r="F500" t="inlineStr">
         <is>
@@ -16454,7 +16454,7 @@
         <v>17700000</v>
       </c>
       <c r="E501" t="n">
-        <v>-647699641</v>
+        <v>647699641</v>
       </c>
       <c r="F501" t="inlineStr">
         <is>
@@ -16486,7 +16486,7 @@
         <v>17700000</v>
       </c>
       <c r="E502" t="n">
-        <v>-98906104</v>
+        <v>98906104</v>
       </c>
       <c r="F502" t="inlineStr">
         <is>
@@ -16518,7 +16518,7 @@
         <v>17700000</v>
       </c>
       <c r="E503" t="n">
-        <v>-850886592</v>
+        <v>850886592</v>
       </c>
       <c r="F503" t="inlineStr">
         <is>
@@ -16550,7 +16550,7 @@
         <v>17700000</v>
       </c>
       <c r="E504" t="n">
-        <v>-193059055</v>
+        <v>193059055</v>
       </c>
       <c r="F504" t="inlineStr">
         <is>
@@ -16678,7 +16678,7 @@
         <v>17600000</v>
       </c>
       <c r="E508" t="n">
-        <v>-2020959773</v>
+        <v>2020959773</v>
       </c>
       <c r="F508" t="inlineStr">
         <is>
@@ -16710,7 +16710,7 @@
         <v>17600000</v>
       </c>
       <c r="E509" t="n">
-        <v>-1317225719</v>
+        <v>1317225719</v>
       </c>
       <c r="F509" t="inlineStr">
         <is>
@@ -16742,7 +16742,7 @@
         <v>17600000</v>
       </c>
       <c r="E510" t="n">
-        <v>-542620034</v>
+        <v>542620034</v>
       </c>
       <c r="F510" t="inlineStr">
         <is>
@@ -16806,7 +16806,7 @@
         <v>17600000</v>
       </c>
       <c r="E512" t="n">
-        <v>-492687198</v>
+        <v>492687198</v>
       </c>
       <c r="F512" t="inlineStr">
         <is>
@@ -16838,7 +16838,7 @@
         <v>17500000</v>
       </c>
       <c r="E513" t="n">
-        <v>-2056832858</v>
+        <v>2056832858</v>
       </c>
       <c r="F513" t="inlineStr">
         <is>
@@ -16870,7 +16870,7 @@
         <v>17500000</v>
       </c>
       <c r="E514" t="n">
-        <v>-1326315016</v>
+        <v>1326315016</v>
       </c>
       <c r="F514" t="inlineStr">
         <is>
@@ -16902,7 +16902,7 @@
         <v>17500000</v>
       </c>
       <c r="E515" t="n">
-        <v>-977548970</v>
+        <v>977548970</v>
       </c>
       <c r="F515" t="inlineStr">
         <is>
@@ -16934,7 +16934,7 @@
         <v>17500000</v>
       </c>
       <c r="E516" t="n">
-        <v>-1072752635</v>
+        <v>1072752635</v>
       </c>
       <c r="F516" t="inlineStr">
         <is>
@@ -17030,7 +17030,7 @@
         <v>17400000</v>
       </c>
       <c r="E519" t="n">
-        <v>-1740706424</v>
+        <v>1740706424</v>
       </c>
       <c r="F519" t="inlineStr">
         <is>
@@ -17062,7 +17062,7 @@
         <v>17400000</v>
       </c>
       <c r="E520" t="n">
-        <v>-619311696</v>
+        <v>619311696</v>
       </c>
       <c r="F520" t="inlineStr">
         <is>
@@ -17158,7 +17158,7 @@
         <v>17300000</v>
       </c>
       <c r="E523" t="n">
-        <v>-1513163841</v>
+        <v>1513163841</v>
       </c>
       <c r="F523" t="inlineStr">
         <is>
@@ -17190,7 +17190,7 @@
         <v>17300000</v>
       </c>
       <c r="E524" t="n">
-        <v>-610151137</v>
+        <v>610151137</v>
       </c>
       <c r="F524" t="inlineStr">
         <is>
@@ -17254,7 +17254,7 @@
         <v>17200000</v>
       </c>
       <c r="E526" t="n">
-        <v>-688054825</v>
+        <v>688054825</v>
       </c>
       <c r="F526" t="inlineStr">
         <is>
@@ -17286,7 +17286,7 @@
         <v>17200000</v>
       </c>
       <c r="E527" t="n">
-        <v>-1252722011</v>
+        <v>1252722011</v>
       </c>
       <c r="F527" t="inlineStr">
         <is>
@@ -17350,7 +17350,7 @@
         <v>17200000</v>
       </c>
       <c r="E529" t="n">
-        <v>-1439409484</v>
+        <v>1439409484</v>
       </c>
       <c r="F529" t="inlineStr">
         <is>
@@ -17478,7 +17478,7 @@
         <v>17100000</v>
       </c>
       <c r="E533" t="n">
-        <v>-2121861134</v>
+        <v>2121861134</v>
       </c>
       <c r="F533" t="inlineStr">
         <is>
@@ -17510,7 +17510,7 @@
         <v>17000000</v>
       </c>
       <c r="E534" t="n">
-        <v>-2036953056</v>
+        <v>2036953056</v>
       </c>
       <c r="F534" t="inlineStr">
         <is>
@@ -17574,7 +17574,7 @@
         <v>17000000</v>
       </c>
       <c r="E536" t="n">
-        <v>-360051478</v>
+        <v>360051478</v>
       </c>
       <c r="F536" t="inlineStr">
         <is>
@@ -17702,7 +17702,7 @@
         <v>16900000</v>
       </c>
       <c r="E540" t="n">
-        <v>-467060422</v>
+        <v>467060422</v>
       </c>
       <c r="F540" t="inlineStr">
         <is>
@@ -17830,7 +17830,7 @@
         <v>16900000</v>
       </c>
       <c r="E544" t="n">
-        <v>-771388631</v>
+        <v>771388631</v>
       </c>
       <c r="F544" t="inlineStr">
         <is>
@@ -17862,7 +17862,7 @@
         <v>16800000</v>
       </c>
       <c r="E545" t="n">
-        <v>-1979004978</v>
+        <v>1979004978</v>
       </c>
       <c r="F545" t="inlineStr">
         <is>
@@ -17894,7 +17894,7 @@
         <v>16800000</v>
       </c>
       <c r="E546" t="n">
-        <v>-2071516091</v>
+        <v>2071516091</v>
       </c>
       <c r="F546" t="inlineStr">
         <is>
@@ -17926,7 +17926,7 @@
         <v>16800000</v>
       </c>
       <c r="E547" t="n">
-        <v>-1383471879</v>
+        <v>1383471879</v>
       </c>
       <c r="F547" t="inlineStr">
         <is>
@@ -17958,7 +17958,7 @@
         <v>16800000</v>
       </c>
       <c r="E548" t="n">
-        <v>-1394619792</v>
+        <v>1394619792</v>
       </c>
       <c r="F548" t="inlineStr">
         <is>
@@ -17990,7 +17990,7 @@
         <v>16800000</v>
       </c>
       <c r="E549" t="n">
-        <v>-601168492</v>
+        <v>601168492</v>
       </c>
       <c r="F549" t="inlineStr">
         <is>
@@ -18054,7 +18054,7 @@
         <v>16700000</v>
       </c>
       <c r="E551" t="n">
-        <v>-1486968971</v>
+        <v>1486968971</v>
       </c>
       <c r="F551" t="inlineStr">
         <is>
@@ -18118,7 +18118,7 @@
         <v>16700000</v>
       </c>
       <c r="E553" t="n">
-        <v>-610198011</v>
+        <v>610198011</v>
       </c>
       <c r="F553" t="inlineStr">
         <is>
@@ -18214,7 +18214,7 @@
         <v>16600000</v>
       </c>
       <c r="E556" t="n">
-        <v>-1496693334</v>
+        <v>1496693334</v>
       </c>
       <c r="F556" t="inlineStr">
         <is>
@@ -18246,7 +18246,7 @@
         <v>16600000</v>
       </c>
       <c r="E557" t="n">
-        <v>-597993840</v>
+        <v>597993840</v>
       </c>
       <c r="F557" t="inlineStr">
         <is>
@@ -18278,7 +18278,7 @@
         <v>16600000</v>
       </c>
       <c r="E558" t="n">
-        <v>-1154753765</v>
+        <v>1154753765</v>
       </c>
       <c r="F558" t="inlineStr">
         <is>
@@ -18342,7 +18342,7 @@
         <v>16600000</v>
       </c>
       <c r="E560" t="n">
-        <v>-938684028</v>
+        <v>938684028</v>
       </c>
       <c r="F560" t="inlineStr">
         <is>
@@ -18374,7 +18374,7 @@
         <v>16600000</v>
       </c>
       <c r="E561" t="n">
-        <v>-1901200327</v>
+        <v>1901200327</v>
       </c>
       <c r="F561" t="inlineStr">
         <is>
@@ -18438,7 +18438,7 @@
         <v>16500000</v>
       </c>
       <c r="E563" t="n">
-        <v>-1854033262</v>
+        <v>1854033262</v>
       </c>
       <c r="F563" t="inlineStr">
         <is>
@@ -18470,7 +18470,7 @@
         <v>16500000</v>
       </c>
       <c r="E564" t="n">
-        <v>-1257706616</v>
+        <v>1257706616</v>
       </c>
       <c r="F564" t="inlineStr">
         <is>
@@ -18502,7 +18502,7 @@
         <v>16500000</v>
       </c>
       <c r="E565" t="n">
-        <v>-1546699461</v>
+        <v>1546699461</v>
       </c>
       <c r="F565" t="inlineStr">
         <is>
@@ -18534,7 +18534,7 @@
         <v>16500000</v>
       </c>
       <c r="E566" t="n">
-        <v>-1183726662</v>
+        <v>1183726662</v>
       </c>
       <c r="F566" t="inlineStr">
         <is>
@@ -18566,7 +18566,7 @@
         <v>16400000</v>
       </c>
       <c r="E567" t="n">
-        <v>-339541137</v>
+        <v>339541137</v>
       </c>
       <c r="F567" t="inlineStr">
         <is>
@@ -18630,7 +18630,7 @@
         <v>16400000</v>
       </c>
       <c r="E569" t="n">
-        <v>-1454113871</v>
+        <v>1454113871</v>
       </c>
       <c r="F569" t="inlineStr">
         <is>
@@ -18758,7 +18758,7 @@
         <v>16400000</v>
       </c>
       <c r="E573" t="n">
-        <v>-40469547</v>
+        <v>40469547</v>
       </c>
       <c r="F573" t="inlineStr">
         <is>
@@ -18790,7 +18790,7 @@
         <v>16300000</v>
       </c>
       <c r="E574" t="n">
-        <v>-767340032</v>
+        <v>767340032</v>
       </c>
       <c r="F574" t="inlineStr">
         <is>
@@ -18822,7 +18822,7 @@
         <v>16300000</v>
       </c>
       <c r="E575" t="n">
-        <v>-2011106445</v>
+        <v>2011106445</v>
       </c>
       <c r="F575" t="inlineStr">
         <is>
@@ -18854,7 +18854,7 @@
         <v>16300000</v>
       </c>
       <c r="E576" t="n">
-        <v>-1976511957</v>
+        <v>1976511957</v>
       </c>
       <c r="F576" t="inlineStr">
         <is>
@@ -18886,7 +18886,7 @@
         <v>16300000</v>
       </c>
       <c r="E577" t="n">
-        <v>-1069691966</v>
+        <v>1069691966</v>
       </c>
       <c r="F577" t="inlineStr">
         <is>
@@ -18950,7 +18950,7 @@
         <v>16300000</v>
       </c>
       <c r="E579" t="n">
-        <v>-409187506</v>
+        <v>409187506</v>
       </c>
       <c r="F579" t="inlineStr">
         <is>
@@ -18982,7 +18982,7 @@
         <v>16300000</v>
       </c>
       <c r="E580" t="n">
-        <v>-1448109325</v>
+        <v>1448109325</v>
       </c>
       <c r="F580" t="inlineStr">
         <is>
@@ -19110,7 +19110,7 @@
         <v>16200000</v>
       </c>
       <c r="E584" t="n">
-        <v>-498228360</v>
+        <v>498228360</v>
       </c>
       <c r="F584" t="inlineStr">
         <is>
@@ -19142,7 +19142,7 @@
         <v>16200000</v>
       </c>
       <c r="E585" t="n">
-        <v>-1304781829</v>
+        <v>1304781829</v>
       </c>
       <c r="F585" t="inlineStr">
         <is>
@@ -19174,7 +19174,7 @@
         <v>16200000</v>
       </c>
       <c r="E586" t="n">
-        <v>-218274673</v>
+        <v>218274673</v>
       </c>
       <c r="F586" t="inlineStr">
         <is>
@@ -19270,7 +19270,7 @@
         <v>16200000</v>
       </c>
       <c r="E589" t="n">
-        <v>-952497381</v>
+        <v>952497381</v>
       </c>
       <c r="F589" t="inlineStr">
         <is>
@@ -19462,7 +19462,7 @@
         <v>16100000</v>
       </c>
       <c r="E595" t="n">
-        <v>-1190638587</v>
+        <v>1190638587</v>
       </c>
       <c r="F595" t="inlineStr">
         <is>
@@ -19494,7 +19494,7 @@
         <v>16100000</v>
       </c>
       <c r="E596" t="n">
-        <v>-1607523653</v>
+        <v>1607523653</v>
       </c>
       <c r="F596" t="inlineStr">
         <is>
@@ -19558,7 +19558,7 @@
         <v>16100000</v>
       </c>
       <c r="E598" t="n">
-        <v>-1717231802</v>
+        <v>1717231802</v>
       </c>
       <c r="F598" t="inlineStr">
         <is>
@@ -19590,7 +19590,7 @@
         <v>16100000</v>
       </c>
       <c r="E599" t="n">
-        <v>-1463723871</v>
+        <v>1463723871</v>
       </c>
       <c r="F599" t="inlineStr">
         <is>
@@ -19622,7 +19622,7 @@
         <v>16100000</v>
       </c>
       <c r="E600" t="n">
-        <v>-1434198586</v>
+        <v>1434198586</v>
       </c>
       <c r="F600" t="inlineStr">
         <is>
@@ -19654,7 +19654,7 @@
         <v>16100000</v>
       </c>
       <c r="E601" t="n">
-        <v>-1367859888</v>
+        <v>1367859888</v>
       </c>
       <c r="F601" t="inlineStr">
         <is>
@@ -19718,7 +19718,7 @@
         <v>16000000</v>
       </c>
       <c r="E603" t="n">
-        <v>-2046304913</v>
+        <v>2046304913</v>
       </c>
       <c r="F603" t="inlineStr">
         <is>
@@ -19750,7 +19750,7 @@
         <v>16000000</v>
       </c>
       <c r="E604" t="n">
-        <v>-1276934873</v>
+        <v>1276934873</v>
       </c>
       <c r="F604" t="inlineStr">
         <is>
@@ -19782,7 +19782,7 @@
         <v>16000000</v>
       </c>
       <c r="E605" t="n">
-        <v>-1265094388</v>
+        <v>1265094388</v>
       </c>
       <c r="F605" t="inlineStr">
         <is>
@@ -19942,7 +19942,7 @@
         <v>15900000</v>
       </c>
       <c r="E610" t="n">
-        <v>-1685608828</v>
+        <v>1685608828</v>
       </c>
       <c r="F610" t="inlineStr">
         <is>
@@ -19974,7 +19974,7 @@
         <v>15900000</v>
       </c>
       <c r="E611" t="n">
-        <v>-2055608180</v>
+        <v>2055608180</v>
       </c>
       <c r="F611" t="inlineStr">
         <is>
@@ -20070,7 +20070,7 @@
         <v>15900000</v>
       </c>
       <c r="E614" t="n">
-        <v>-1787552113</v>
+        <v>1787552113</v>
       </c>
       <c r="F614" t="inlineStr">
         <is>
@@ -20134,7 +20134,7 @@
         <v>15800000</v>
       </c>
       <c r="E616" t="n">
-        <v>-902048307</v>
+        <v>902048307</v>
       </c>
       <c r="F616" t="inlineStr">
         <is>
@@ -20166,7 +20166,7 @@
         <v>15800000</v>
       </c>
       <c r="E617" t="n">
-        <v>-172332829</v>
+        <v>172332829</v>
       </c>
       <c r="F617" t="inlineStr">
         <is>
@@ -20326,7 +20326,7 @@
         <v>15700000</v>
       </c>
       <c r="E622" t="n">
-        <v>-1963371084</v>
+        <v>1963371084</v>
       </c>
       <c r="F622" t="inlineStr">
         <is>
@@ -20454,7 +20454,7 @@
         <v>15600000</v>
       </c>
       <c r="E626" t="n">
-        <v>-1727405176</v>
+        <v>1727405176</v>
       </c>
       <c r="F626" t="inlineStr">
         <is>
@@ -20486,7 +20486,7 @@
         <v>15600000</v>
       </c>
       <c r="E627" t="n">
-        <v>-1417548083</v>
+        <v>1417548083</v>
       </c>
       <c r="F627" t="inlineStr">
         <is>
@@ -20518,7 +20518,7 @@
         <v>15600000</v>
       </c>
       <c r="E628" t="n">
-        <v>-425510199</v>
+        <v>425510199</v>
       </c>
       <c r="F628" t="inlineStr">
         <is>
@@ -20678,7 +20678,7 @@
         <v>15500000</v>
       </c>
       <c r="E633" t="n">
-        <v>-813228408</v>
+        <v>813228408</v>
       </c>
       <c r="F633" t="inlineStr">
         <is>
@@ -20710,7 +20710,7 @@
         <v>15500000</v>
       </c>
       <c r="E634" t="n">
-        <v>-324804953</v>
+        <v>324804953</v>
       </c>
       <c r="F634" t="inlineStr">
         <is>
@@ -20774,7 +20774,7 @@
         <v>15500000</v>
       </c>
       <c r="E636" t="n">
-        <v>-4513635</v>
+        <v>4513635</v>
       </c>
       <c r="F636" t="inlineStr">
         <is>
@@ -20806,7 +20806,7 @@
         <v>15500000</v>
       </c>
       <c r="E637" t="n">
-        <v>-170760148</v>
+        <v>170760148</v>
       </c>
       <c r="F637" t="inlineStr">
         <is>
@@ -20934,7 +20934,7 @@
         <v>15400000</v>
       </c>
       <c r="E641" t="n">
-        <v>-1371162981</v>
+        <v>1371162981</v>
       </c>
       <c r="F641" t="inlineStr">
         <is>
@@ -21030,7 +21030,7 @@
         <v>15400000</v>
       </c>
       <c r="E644" t="n">
-        <v>-558897316</v>
+        <v>558897316</v>
       </c>
       <c r="F644" t="inlineStr">
         <is>
@@ -21158,7 +21158,7 @@
         <v>15300000</v>
       </c>
       <c r="E648" t="n">
-        <v>-1638439091</v>
+        <v>1638439091</v>
       </c>
       <c r="F648" t="inlineStr">
         <is>
@@ -21286,7 +21286,7 @@
         <v>15300000</v>
       </c>
       <c r="E652" t="n">
-        <v>-633903052</v>
+        <v>633903052</v>
       </c>
       <c r="F652" t="inlineStr">
         <is>
@@ -21446,7 +21446,7 @@
         <v>15200000</v>
       </c>
       <c r="E657" t="n">
-        <v>-1438251095</v>
+        <v>1438251095</v>
       </c>
       <c r="F657" t="inlineStr">
         <is>
@@ -21478,7 +21478,7 @@
         <v>15200000</v>
       </c>
       <c r="E658" t="n">
-        <v>-1025281944</v>
+        <v>1025281944</v>
       </c>
       <c r="F658" t="inlineStr">
         <is>
@@ -21510,7 +21510,7 @@
         <v>15200000</v>
       </c>
       <c r="E659" t="n">
-        <v>-256546807</v>
+        <v>256546807</v>
       </c>
       <c r="F659" t="inlineStr">
         <is>
@@ -21574,7 +21574,7 @@
         <v>15200000</v>
       </c>
       <c r="E661" t="n">
-        <v>-1965766437</v>
+        <v>1965766437</v>
       </c>
       <c r="F661" t="inlineStr">
         <is>
@@ -21702,7 +21702,7 @@
         <v>15100000</v>
       </c>
       <c r="E665" t="n">
-        <v>-1894929734</v>
+        <v>1894929734</v>
       </c>
       <c r="F665" t="inlineStr">
         <is>
@@ -21766,7 +21766,7 @@
         <v>15100000</v>
       </c>
       <c r="E667" t="n">
-        <v>-1234764449</v>
+        <v>1234764449</v>
       </c>
       <c r="F667" t="inlineStr">
         <is>
@@ -21798,7 +21798,7 @@
         <v>15100000</v>
       </c>
       <c r="E668" t="n">
-        <v>-1533419538</v>
+        <v>1533419538</v>
       </c>
       <c r="F668" t="inlineStr">
         <is>
@@ -21830,7 +21830,7 @@
         <v>15100000</v>
       </c>
       <c r="E669" t="n">
-        <v>-58931155</v>
+        <v>58931155</v>
       </c>
       <c r="F669" t="inlineStr">
         <is>
@@ -21926,7 +21926,7 @@
         <v>15100000</v>
       </c>
       <c r="E672" t="n">
-        <v>-1921426736</v>
+        <v>1921426736</v>
       </c>
       <c r="F672" t="inlineStr">
         <is>
@@ -21958,7 +21958,7 @@
         <v>15100000</v>
       </c>
       <c r="E673" t="n">
-        <v>-732562822</v>
+        <v>732562822</v>
       </c>
       <c r="F673" t="inlineStr">
         <is>
@@ -22086,7 +22086,7 @@
         <v>15100000</v>
       </c>
       <c r="E677" t="n">
-        <v>-471032007</v>
+        <v>471032007</v>
       </c>
       <c r="F677" t="inlineStr">
         <is>
@@ -22214,7 +22214,7 @@
         <v>15000000</v>
       </c>
       <c r="E681" t="n">
-        <v>-1430183622</v>
+        <v>1430183622</v>
       </c>
       <c r="F681" t="inlineStr">
         <is>
@@ -22246,7 +22246,7 @@
         <v>15000000</v>
       </c>
       <c r="E682" t="n">
-        <v>-1564088272</v>
+        <v>1564088272</v>
       </c>
       <c r="F682" t="inlineStr">
         <is>
@@ -22278,7 +22278,7 @@
         <v>15000000</v>
       </c>
       <c r="E683" t="n">
-        <v>-286165423</v>
+        <v>286165423</v>
       </c>
       <c r="F683" t="inlineStr">
         <is>
@@ -22342,7 +22342,7 @@
         <v>15000000</v>
       </c>
       <c r="E685" t="n">
-        <v>-1700630286</v>
+        <v>1700630286</v>
       </c>
       <c r="F685" t="inlineStr">
         <is>
@@ -22374,7 +22374,7 @@
         <v>15000000</v>
       </c>
       <c r="E686" t="n">
-        <v>-1053841527</v>
+        <v>1053841527</v>
       </c>
       <c r="F686" t="inlineStr">
         <is>
@@ -22534,7 +22534,7 @@
         <v>15000000</v>
       </c>
       <c r="E691" t="n">
-        <v>-1057591067</v>
+        <v>1057591067</v>
       </c>
       <c r="F691" t="inlineStr">
         <is>
@@ -22598,7 +22598,7 @@
         <v>15000000</v>
       </c>
       <c r="E693" t="n">
-        <v>-1378199256</v>
+        <v>1378199256</v>
       </c>
       <c r="F693" t="inlineStr">
         <is>
@@ -22694,7 +22694,7 @@
         <v>14900000</v>
       </c>
       <c r="E696" t="n">
-        <v>-515673614</v>
+        <v>515673614</v>
       </c>
       <c r="F696" t="inlineStr">
         <is>
@@ -22726,7 +22726,7 @@
         <v>14900000</v>
       </c>
       <c r="E697" t="n">
-        <v>-261567129</v>
+        <v>261567129</v>
       </c>
       <c r="F697" t="inlineStr">
         <is>
@@ -22854,7 +22854,7 @@
         <v>14900000</v>
       </c>
       <c r="E701" t="n">
-        <v>-1266548189</v>
+        <v>1266548189</v>
       </c>
       <c r="F701" t="inlineStr">
         <is>
@@ -23046,7 +23046,7 @@
         <v>14800000</v>
       </c>
       <c r="E707" t="n">
-        <v>-707390512</v>
+        <v>707390512</v>
       </c>
       <c r="F707" t="inlineStr">
         <is>
@@ -23110,7 +23110,7 @@
         <v>14800000</v>
       </c>
       <c r="E709" t="n">
-        <v>-1571919530</v>
+        <v>1571919530</v>
       </c>
       <c r="F709" t="inlineStr">
         <is>
@@ -23270,7 +23270,7 @@
         <v>14800000</v>
       </c>
       <c r="E714" t="n">
-        <v>-1391660662</v>
+        <v>1391660662</v>
       </c>
       <c r="F714" t="inlineStr">
         <is>
@@ -23334,7 +23334,7 @@
         <v>14700000</v>
       </c>
       <c r="E716" t="n">
-        <v>-2063981257</v>
+        <v>2063981257</v>
       </c>
       <c r="F716" t="inlineStr">
         <is>
@@ -23430,7 +23430,7 @@
         <v>14700000</v>
       </c>
       <c r="E719" t="n">
-        <v>-1829493524</v>
+        <v>1829493524</v>
       </c>
       <c r="F719" t="inlineStr">
         <is>
@@ -23462,7 +23462,7 @@
         <v>14700000</v>
       </c>
       <c r="E720" t="n">
-        <v>-265713629</v>
+        <v>265713629</v>
       </c>
       <c r="F720" t="inlineStr">
         <is>
@@ -23494,7 +23494,7 @@
         <v>14700000</v>
       </c>
       <c r="E721" t="n">
-        <v>-1837948604</v>
+        <v>1837948604</v>
       </c>
       <c r="F721" t="inlineStr">
         <is>
@@ -23526,7 +23526,7 @@
         <v>14700000</v>
       </c>
       <c r="E722" t="n">
-        <v>-1334086467</v>
+        <v>1334086467</v>
       </c>
       <c r="F722" t="inlineStr">
         <is>
@@ -23590,7 +23590,7 @@
         <v>14700000</v>
       </c>
       <c r="E724" t="n">
-        <v>-522570359</v>
+        <v>522570359</v>
       </c>
       <c r="F724" t="inlineStr">
         <is>
@@ -23686,7 +23686,7 @@
         <v>14600000</v>
       </c>
       <c r="E727" t="n">
-        <v>-1681769849</v>
+        <v>1681769849</v>
       </c>
       <c r="F727" t="inlineStr">
         <is>
@@ -23718,7 +23718,7 @@
         <v>14600000</v>
       </c>
       <c r="E728" t="n">
-        <v>-957892376</v>
+        <v>957892376</v>
       </c>
       <c r="F728" t="inlineStr">
         <is>
@@ -23750,7 +23750,7 @@
         <v>14600000</v>
       </c>
       <c r="E729" t="n">
-        <v>-691411089</v>
+        <v>691411089</v>
       </c>
       <c r="F729" t="inlineStr">
         <is>
@@ -23878,7 +23878,7 @@
         <v>14600000</v>
       </c>
       <c r="E733" t="n">
-        <v>-1702599571</v>
+        <v>1702599571</v>
       </c>
       <c r="F733" t="inlineStr">
         <is>
@@ -23910,7 +23910,7 @@
         <v>14600000</v>
       </c>
       <c r="E734" t="n">
-        <v>-637665666</v>
+        <v>637665666</v>
       </c>
       <c r="F734" t="inlineStr">
         <is>
@@ -23942,7 +23942,7 @@
         <v>14600000</v>
       </c>
       <c r="E735" t="n">
-        <v>-1544064530</v>
+        <v>1544064530</v>
       </c>
       <c r="F735" t="inlineStr">
         <is>
@@ -24006,7 +24006,7 @@
         <v>14500000</v>
       </c>
       <c r="E737" t="n">
-        <v>-1854249207</v>
+        <v>1854249207</v>
       </c>
       <c r="F737" t="inlineStr">
         <is>
@@ -24038,7 +24038,7 @@
         <v>14500000</v>
       </c>
       <c r="E738" t="n">
-        <v>-1644967011</v>
+        <v>1644967011</v>
       </c>
       <c r="F738" t="inlineStr">
         <is>
@@ -24134,7 +24134,7 @@
         <v>14500000</v>
       </c>
       <c r="E741" t="n">
-        <v>-743077339</v>
+        <v>743077339</v>
       </c>
       <c r="F741" t="inlineStr">
         <is>
@@ -24166,7 +24166,7 @@
         <v>14500000</v>
       </c>
       <c r="E742" t="n">
-        <v>-34779368</v>
+        <v>34779368</v>
       </c>
       <c r="F742" t="inlineStr">
         <is>
@@ -24326,7 +24326,7 @@
         <v>14500000</v>
       </c>
       <c r="E747" t="n">
-        <v>-7238435</v>
+        <v>7238435</v>
       </c>
       <c r="F747" t="inlineStr">
         <is>
@@ -24422,7 +24422,7 @@
         <v>14500000</v>
       </c>
       <c r="E750" t="n">
-        <v>-1432264981</v>
+        <v>1432264981</v>
       </c>
       <c r="F750" t="inlineStr">
         <is>
@@ -24518,7 +24518,7 @@
         <v>14500000</v>
       </c>
       <c r="E753" t="n">
-        <v>-777304876</v>
+        <v>777304876</v>
       </c>
       <c r="F753" t="inlineStr">
         <is>
@@ -24582,7 +24582,7 @@
         <v>14400000</v>
       </c>
       <c r="E755" t="n">
-        <v>-2070845406</v>
+        <v>2070845406</v>
       </c>
       <c r="F755" t="inlineStr">
         <is>
@@ -24678,7 +24678,7 @@
         <v>14400000</v>
       </c>
       <c r="E758" t="n">
-        <v>-1322493081</v>
+        <v>1322493081</v>
       </c>
       <c r="F758" t="inlineStr">
         <is>
@@ -24710,7 +24710,7 @@
         <v>14400000</v>
       </c>
       <c r="E759" t="n">
-        <v>-1208712751</v>
+        <v>1208712751</v>
       </c>
       <c r="F759" t="inlineStr">
         <is>
@@ -24742,7 +24742,7 @@
         <v>14400000</v>
       </c>
       <c r="E760" t="n">
-        <v>-394654665</v>
+        <v>394654665</v>
       </c>
       <c r="F760" t="inlineStr">
         <is>
@@ -24774,7 +24774,7 @@
         <v>14400000</v>
       </c>
       <c r="E761" t="n">
-        <v>-259228565</v>
+        <v>259228565</v>
       </c>
       <c r="F761" t="inlineStr">
         <is>
@@ -24806,7 +24806,7 @@
         <v>14400000</v>
       </c>
       <c r="E762" t="n">
-        <v>-138539499</v>
+        <v>138539499</v>
       </c>
       <c r="F762" t="inlineStr">
         <is>
@@ -24902,7 +24902,7 @@
         <v>14400000</v>
       </c>
       <c r="E765" t="n">
-        <v>-2046652133</v>
+        <v>2046652133</v>
       </c>
       <c r="F765" t="inlineStr">
         <is>
@@ -24934,7 +24934,7 @@
         <v>14400000</v>
       </c>
       <c r="E766" t="n">
-        <v>-577957304</v>
+        <v>577957304</v>
       </c>
       <c r="F766" t="inlineStr">
         <is>
@@ -24998,7 +24998,7 @@
         <v>14400000</v>
       </c>
       <c r="E768" t="n">
-        <v>-1461108919</v>
+        <v>1461108919</v>
       </c>
       <c r="F768" t="inlineStr">
         <is>
@@ -25158,7 +25158,7 @@
         <v>14200000</v>
       </c>
       <c r="E773" t="n">
-        <v>-254670290</v>
+        <v>254670290</v>
       </c>
       <c r="F773" t="inlineStr">
         <is>
@@ -25190,7 +25190,7 @@
         <v>14200000</v>
       </c>
       <c r="E774" t="n">
-        <v>-1616002039</v>
+        <v>1616002039</v>
       </c>
       <c r="F774" t="inlineStr">
         <is>
@@ -25286,7 +25286,7 @@
         <v>14200000</v>
       </c>
       <c r="E777" t="n">
-        <v>-374407744</v>
+        <v>374407744</v>
       </c>
       <c r="F777" t="inlineStr">
         <is>
@@ -25318,7 +25318,7 @@
         <v>14200000</v>
       </c>
       <c r="E778" t="n">
-        <v>-2035934272</v>
+        <v>2035934272</v>
       </c>
       <c r="F778" t="inlineStr">
         <is>
@@ -25350,7 +25350,7 @@
         <v>14200000</v>
       </c>
       <c r="E779" t="n">
-        <v>-643612531</v>
+        <v>643612531</v>
       </c>
       <c r="F779" t="inlineStr">
         <is>
@@ -25446,7 +25446,7 @@
         <v>14200000</v>
       </c>
       <c r="E782" t="n">
-        <v>-1456107061</v>
+        <v>1456107061</v>
       </c>
       <c r="F782" t="inlineStr">
         <is>
@@ -25478,7 +25478,7 @@
         <v>14200000</v>
       </c>
       <c r="E783" t="n">
-        <v>-977161753</v>
+        <v>977161753</v>
       </c>
       <c r="F783" t="inlineStr">
         <is>
@@ -25542,7 +25542,7 @@
         <v>14100000</v>
       </c>
       <c r="E785" t="n">
-        <v>-700030521</v>
+        <v>700030521</v>
       </c>
       <c r="F785" t="inlineStr">
         <is>
@@ -25574,7 +25574,7 @@
         <v>14100000</v>
       </c>
       <c r="E786" t="n">
-        <v>-374745974</v>
+        <v>374745974</v>
       </c>
       <c r="F786" t="inlineStr">
         <is>
@@ -25702,7 +25702,7 @@
         <v>14100000</v>
       </c>
       <c r="E790" t="n">
-        <v>-1705719300</v>
+        <v>1705719300</v>
       </c>
       <c r="F790" t="inlineStr">
         <is>
@@ -25766,7 +25766,7 @@
         <v>14100000</v>
       </c>
       <c r="E792" t="n">
-        <v>-1014485369</v>
+        <v>1014485369</v>
       </c>
       <c r="F792" t="inlineStr">
         <is>
@@ -25862,7 +25862,7 @@
         <v>14000000</v>
       </c>
       <c r="E795" t="n">
-        <v>-2080799450</v>
+        <v>2080799450</v>
       </c>
       <c r="F795" t="inlineStr">
         <is>
@@ -25926,7 +25926,7 @@
         <v>14000000</v>
       </c>
       <c r="E797" t="n">
-        <v>-870191480</v>
+        <v>870191480</v>
       </c>
       <c r="F797" t="inlineStr">
         <is>
@@ -26086,7 +26086,7 @@
         <v>14000000</v>
       </c>
       <c r="E802" t="n">
-        <v>-287834756</v>
+        <v>287834756</v>
       </c>
       <c r="F802" t="inlineStr">
         <is>
@@ -26214,7 +26214,7 @@
         <v>13900000</v>
       </c>
       <c r="E806" t="n">
-        <v>-2050648916</v>
+        <v>2050648916</v>
       </c>
       <c r="F806" t="inlineStr">
         <is>
@@ -26246,7 +26246,7 @@
         <v>13900000</v>
       </c>
       <c r="E807" t="n">
-        <v>-1139588872</v>
+        <v>1139588872</v>
       </c>
       <c r="F807" t="inlineStr">
         <is>
@@ -26342,7 +26342,7 @@
         <v>13900000</v>
       </c>
       <c r="E810" t="n">
-        <v>-755318833</v>
+        <v>755318833</v>
       </c>
       <c r="F810" t="inlineStr">
         <is>
@@ -26374,7 +26374,7 @@
         <v>13900000</v>
       </c>
       <c r="E811" t="n">
-        <v>-371059545</v>
+        <v>371059545</v>
       </c>
       <c r="F811" t="inlineStr">
         <is>
@@ -26406,7 +26406,7 @@
         <v>13900000</v>
       </c>
       <c r="E812" t="n">
-        <v>-138179823</v>
+        <v>138179823</v>
       </c>
       <c r="F812" t="inlineStr">
         <is>
@@ -26438,7 +26438,7 @@
         <v>13900000</v>
       </c>
       <c r="E813" t="n">
-        <v>-2129081662</v>
+        <v>2129081662</v>
       </c>
       <c r="F813" t="inlineStr">
         <is>
@@ -26470,7 +26470,7 @@
         <v>13900000</v>
       </c>
       <c r="E814" t="n">
-        <v>-1101741224</v>
+        <v>1101741224</v>
       </c>
       <c r="F814" t="inlineStr">
         <is>
@@ -26502,7 +26502,7 @@
         <v>13800000</v>
       </c>
       <c r="E815" t="n">
-        <v>-2070056266</v>
+        <v>2070056266</v>
       </c>
       <c r="F815" t="inlineStr">
         <is>
@@ -26598,7 +26598,7 @@
         <v>13800000</v>
       </c>
       <c r="E818" t="n">
-        <v>-1814009614</v>
+        <v>1814009614</v>
       </c>
       <c r="F818" t="inlineStr">
         <is>
@@ -26694,7 +26694,7 @@
         <v>13800000</v>
       </c>
       <c r="E821" t="n">
-        <v>-1942981196</v>
+        <v>1942981196</v>
       </c>
       <c r="F821" t="inlineStr">
         <is>
@@ -26726,7 +26726,7 @@
         <v>13800000</v>
       </c>
       <c r="E822" t="n">
-        <v>-1845558325</v>
+        <v>1845558325</v>
       </c>
       <c r="F822" t="inlineStr">
         <is>
@@ -26886,7 +26886,7 @@
         <v>13700000</v>
       </c>
       <c r="E827" t="n">
-        <v>-1355765910</v>
+        <v>1355765910</v>
       </c>
       <c r="F827" t="inlineStr">
         <is>
@@ -26982,7 +26982,7 @@
         <v>13700000</v>
       </c>
       <c r="E830" t="n">
-        <v>-455555216</v>
+        <v>455555216</v>
       </c>
       <c r="F830" t="inlineStr">
         <is>
@@ -27174,7 +27174,7 @@
         <v>13600000</v>
       </c>
       <c r="E836" t="n">
-        <v>-530358940</v>
+        <v>530358940</v>
       </c>
       <c r="F836" t="inlineStr">
         <is>
@@ -27366,7 +27366,7 @@
         <v>13500000</v>
       </c>
       <c r="E842" t="n">
-        <v>-849173173</v>
+        <v>849173173</v>
       </c>
       <c r="F842" t="inlineStr">
         <is>
@@ -27462,7 +27462,7 @@
         <v>13500000</v>
       </c>
       <c r="E845" t="n">
-        <v>-324013933</v>
+        <v>324013933</v>
       </c>
       <c r="F845" t="inlineStr">
         <is>
@@ -27494,7 +27494,7 @@
         <v>13500000</v>
       </c>
       <c r="E846" t="n">
-        <v>-382632937</v>
+        <v>382632937</v>
       </c>
       <c r="F846" t="inlineStr">
         <is>
@@ -27526,7 +27526,7 @@
         <v>13500000</v>
       </c>
       <c r="E847" t="n">
-        <v>-1167684595</v>
+        <v>1167684595</v>
       </c>
       <c r="F847" t="inlineStr">
         <is>
@@ -27558,7 +27558,7 @@
         <v>13500000</v>
       </c>
       <c r="E848" t="n">
-        <v>-631162720</v>
+        <v>631162720</v>
       </c>
       <c r="F848" t="inlineStr">
         <is>
@@ -27590,7 +27590,7 @@
         <v>13500000</v>
       </c>
       <c r="E849" t="n">
-        <v>-1543973904</v>
+        <v>1543973904</v>
       </c>
       <c r="F849" t="inlineStr">
         <is>
@@ -27686,7 +27686,7 @@
         <v>13400000</v>
       </c>
       <c r="E852" t="n">
-        <v>-1095223233</v>
+        <v>1095223233</v>
       </c>
       <c r="F852" t="inlineStr">
         <is>
@@ -27782,7 +27782,7 @@
         <v>13400000</v>
       </c>
       <c r="E855" t="n">
-        <v>-1644906085</v>
+        <v>1644906085</v>
       </c>
       <c r="F855" t="inlineStr">
         <is>
@@ -27814,7 +27814,7 @@
         <v>13400000</v>
       </c>
       <c r="E856" t="n">
-        <v>-1975451509</v>
+        <v>1975451509</v>
       </c>
       <c r="F856" t="inlineStr">
         <is>
@@ -27846,7 +27846,7 @@
         <v>13400000</v>
       </c>
       <c r="E857" t="n">
-        <v>-931332373</v>
+        <v>931332373</v>
       </c>
       <c r="F857" t="inlineStr">
         <is>
@@ -28006,7 +28006,7 @@
         <v>13300000</v>
       </c>
       <c r="E862" t="n">
-        <v>-2032276553</v>
+        <v>2032276553</v>
       </c>
       <c r="F862" t="inlineStr">
         <is>
@@ -28070,7 +28070,7 @@
         <v>13300000</v>
       </c>
       <c r="E864" t="n">
-        <v>-995750695</v>
+        <v>995750695</v>
       </c>
       <c r="F864" t="inlineStr">
         <is>
@@ -28102,7 +28102,7 @@
         <v>13300000</v>
       </c>
       <c r="E865" t="n">
-        <v>-930736809</v>
+        <v>930736809</v>
       </c>
       <c r="F865" t="inlineStr">
         <is>
@@ -28134,7 +28134,7 @@
         <v>13300000</v>
       </c>
       <c r="E866" t="n">
-        <v>-561110426</v>
+        <v>561110426</v>
       </c>
       <c r="F866" t="inlineStr">
         <is>
@@ -28166,7 +28166,7 @@
         <v>13300000</v>
       </c>
       <c r="E867" t="n">
-        <v>-117783225</v>
+        <v>117783225</v>
       </c>
       <c r="F867" t="inlineStr">
         <is>
@@ -28198,7 +28198,7 @@
         <v>13300000</v>
       </c>
       <c r="E868" t="n">
-        <v>-2107247372</v>
+        <v>2107247372</v>
       </c>
       <c r="F868" t="inlineStr">
         <is>
@@ -28262,7 +28262,7 @@
         <v>13300000</v>
       </c>
       <c r="E870" t="n">
-        <v>-666033339</v>
+        <v>666033339</v>
       </c>
       <c r="F870" t="inlineStr">
         <is>
@@ -28294,7 +28294,7 @@
         <v>13300000</v>
       </c>
       <c r="E871" t="n">
-        <v>-816390983</v>
+        <v>816390983</v>
       </c>
       <c r="F871" t="inlineStr">
         <is>
@@ -28326,7 +28326,7 @@
         <v>13300000</v>
       </c>
       <c r="E872" t="n">
-        <v>-1183305856</v>
+        <v>1183305856</v>
       </c>
       <c r="F872" t="inlineStr">
         <is>
@@ -28358,7 +28358,7 @@
         <v>13300000</v>
       </c>
       <c r="E873" t="n">
-        <v>-1463691793</v>
+        <v>1463691793</v>
       </c>
       <c r="F873" t="inlineStr">
         <is>
@@ -28390,7 +28390,7 @@
         <v>13300000</v>
       </c>
       <c r="E874" t="n">
-        <v>-165717881</v>
+        <v>165717881</v>
       </c>
       <c r="F874" t="inlineStr">
         <is>
@@ -28550,7 +28550,7 @@
         <v>13200000</v>
       </c>
       <c r="E879" t="n">
-        <v>-726575073</v>
+        <v>726575073</v>
       </c>
       <c r="F879" t="inlineStr">
         <is>
@@ -28582,7 +28582,7 @@
         <v>13200000</v>
       </c>
       <c r="E880" t="n">
-        <v>-505231078</v>
+        <v>505231078</v>
       </c>
       <c r="F880" t="inlineStr">
         <is>
@@ -28614,7 +28614,7 @@
         <v>13200000</v>
       </c>
       <c r="E881" t="n">
-        <v>-89302402</v>
+        <v>89302402</v>
       </c>
       <c r="F881" t="inlineStr">
         <is>
@@ -28710,7 +28710,7 @@
         <v>13200000</v>
       </c>
       <c r="E884" t="n">
-        <v>-731249879</v>
+        <v>731249879</v>
       </c>
       <c r="F884" t="inlineStr">
         <is>
@@ -28838,7 +28838,7 @@
         <v>13100000</v>
       </c>
       <c r="E888" t="n">
-        <v>-2112315832</v>
+        <v>2112315832</v>
       </c>
       <c r="F888" t="inlineStr">
         <is>
@@ -28902,7 +28902,7 @@
         <v>13100000</v>
       </c>
       <c r="E890" t="n">
-        <v>-1561284504</v>
+        <v>1561284504</v>
       </c>
       <c r="F890" t="inlineStr">
         <is>
@@ -29030,7 +29030,7 @@
         <v>13100000</v>
       </c>
       <c r="E894" t="n">
-        <v>-1739165494</v>
+        <v>1739165494</v>
       </c>
       <c r="F894" t="inlineStr">
         <is>
@@ -29062,7 +29062,7 @@
         <v>13100000</v>
       </c>
       <c r="E895" t="n">
-        <v>-80794305</v>
+        <v>80794305</v>
       </c>
       <c r="F895" t="inlineStr">
         <is>
@@ -29158,7 +29158,7 @@
         <v>13100000</v>
       </c>
       <c r="E898" t="n">
-        <v>-1415703380</v>
+        <v>1415703380</v>
       </c>
       <c r="F898" t="inlineStr">
         <is>
@@ -29254,7 +29254,7 @@
         <v>13100000</v>
       </c>
       <c r="E901" t="n">
-        <v>-1952113861</v>
+        <v>1952113861</v>
       </c>
       <c r="F901" t="inlineStr">
         <is>
@@ -29286,7 +29286,7 @@
         <v>13000000</v>
       </c>
       <c r="E902" t="n">
-        <v>-1611669447</v>
+        <v>1611669447</v>
       </c>
       <c r="F902" t="inlineStr">
         <is>
@@ -29702,7 +29702,7 @@
         <v>12900000</v>
       </c>
       <c r="E915" t="n">
-        <v>-1785214352</v>
+        <v>1785214352</v>
       </c>
       <c r="F915" t="inlineStr">
         <is>
@@ -29734,7 +29734,7 @@
         <v>12900000</v>
       </c>
       <c r="E916" t="n">
-        <v>-1116744499</v>
+        <v>1116744499</v>
       </c>
       <c r="F916" t="inlineStr">
         <is>
@@ -29766,7 +29766,7 @@
         <v>12900000</v>
       </c>
       <c r="E917" t="n">
-        <v>-651268792</v>
+        <v>651268792</v>
       </c>
       <c r="F917" t="inlineStr">
         <is>
@@ -29830,7 +29830,7 @@
         <v>12900000</v>
       </c>
       <c r="E919" t="n">
-        <v>-1069554641</v>
+        <v>1069554641</v>
       </c>
       <c r="F919" t="inlineStr">
         <is>
@@ -29862,7 +29862,7 @@
         <v>12900000</v>
       </c>
       <c r="E920" t="n">
-        <v>-1380811068</v>
+        <v>1380811068</v>
       </c>
       <c r="F920" t="inlineStr">
         <is>
@@ -29894,7 +29894,7 @@
         <v>12900000</v>
       </c>
       <c r="E921" t="n">
-        <v>-1733161589</v>
+        <v>1733161589</v>
       </c>
       <c r="F921" t="inlineStr">
         <is>
@@ -29958,7 +29958,7 @@
         <v>12900000</v>
       </c>
       <c r="E923" t="n">
-        <v>-1446500774</v>
+        <v>1446500774</v>
       </c>
       <c r="F923" t="inlineStr">
         <is>
@@ -29990,7 +29990,7 @@
         <v>12800000</v>
       </c>
       <c r="E924" t="n">
-        <v>-662528333</v>
+        <v>662528333</v>
       </c>
       <c r="F924" t="inlineStr">
         <is>
@@ -30054,7 +30054,7 @@
         <v>12800000</v>
       </c>
       <c r="E926" t="n">
-        <v>-1927646456</v>
+        <v>1927646456</v>
       </c>
       <c r="F926" t="inlineStr">
         <is>
@@ -30086,7 +30086,7 @@
         <v>12800000</v>
       </c>
       <c r="E927" t="n">
-        <v>-1785861695</v>
+        <v>1785861695</v>
       </c>
       <c r="F927" t="inlineStr">
         <is>
@@ -30118,7 +30118,7 @@
         <v>12800000</v>
       </c>
       <c r="E928" t="n">
-        <v>-1619035071</v>
+        <v>1619035071</v>
       </c>
       <c r="F928" t="inlineStr">
         <is>
@@ -30182,7 +30182,7 @@
         <v>12800000</v>
       </c>
       <c r="E930" t="n">
-        <v>-713193671</v>
+        <v>713193671</v>
       </c>
       <c r="F930" t="inlineStr">
         <is>
@@ -30310,7 +30310,7 @@
         <v>12700000</v>
       </c>
       <c r="E934" t="n">
-        <v>-28010147</v>
+        <v>28010147</v>
       </c>
       <c r="F934" t="inlineStr">
         <is>
@@ -30534,7 +30534,7 @@
         <v>12700000</v>
       </c>
       <c r="E941" t="n">
-        <v>-1585013026</v>
+        <v>1585013026</v>
       </c>
       <c r="F941" t="inlineStr">
         <is>
@@ -30662,7 +30662,7 @@
         <v>12600000</v>
       </c>
       <c r="E945" t="n">
-        <v>-991371986</v>
+        <v>991371986</v>
       </c>
       <c r="F945" t="inlineStr">
         <is>
@@ -30694,7 +30694,7 @@
         <v>12600000</v>
       </c>
       <c r="E946" t="n">
-        <v>-1142564891</v>
+        <v>1142564891</v>
       </c>
       <c r="F946" t="inlineStr">
         <is>
@@ -30726,7 +30726,7 @@
         <v>12600000</v>
       </c>
       <c r="E947" t="n">
-        <v>-809593621</v>
+        <v>809593621</v>
       </c>
       <c r="F947" t="inlineStr">
         <is>
@@ -30790,7 +30790,7 @@
         <v>12600000</v>
       </c>
       <c r="E949" t="n">
-        <v>-1620756511</v>
+        <v>1620756511</v>
       </c>
       <c r="F949" t="inlineStr">
         <is>
@@ -31014,7 +31014,7 @@
         <v>12500000</v>
       </c>
       <c r="E956" t="n">
-        <v>-1633614138</v>
+        <v>1633614138</v>
       </c>
       <c r="F956" t="inlineStr">
         <is>
@@ -31046,7 +31046,7 @@
         <v>12500000</v>
       </c>
       <c r="E957" t="n">
-        <v>-1311167567</v>
+        <v>1311167567</v>
       </c>
       <c r="F957" t="inlineStr">
         <is>
@@ -31078,7 +31078,7 @@
         <v>12500000</v>
       </c>
       <c r="E958" t="n">
-        <v>-1154084156</v>
+        <v>1154084156</v>
       </c>
       <c r="F958" t="inlineStr">
         <is>
@@ -31110,7 +31110,7 @@
         <v>12500000</v>
       </c>
       <c r="E959" t="n">
-        <v>-131328203</v>
+        <v>131328203</v>
       </c>
       <c r="F959" t="inlineStr">
         <is>
@@ -31238,7 +31238,7 @@
         <v>12500000</v>
       </c>
       <c r="E963" t="n">
-        <v>-1100479141</v>
+        <v>1100479141</v>
       </c>
       <c r="F963" t="inlineStr">
         <is>
@@ -31302,7 +31302,7 @@
         <v>12500000</v>
       </c>
       <c r="E965" t="n">
-        <v>-1332711886</v>
+        <v>1332711886</v>
       </c>
       <c r="F965" t="inlineStr">
         <is>
@@ -31334,7 +31334,7 @@
         <v>12500000</v>
       </c>
       <c r="E966" t="n">
-        <v>-1193820587</v>
+        <v>1193820587</v>
       </c>
       <c r="F966" t="inlineStr">
         <is>
@@ -31366,7 +31366,7 @@
         <v>12500000</v>
       </c>
       <c r="E967" t="n">
-        <v>-489080432</v>
+        <v>489080432</v>
       </c>
       <c r="F967" t="inlineStr">
         <is>
@@ -31526,7 +31526,7 @@
         <v>12400000</v>
       </c>
       <c r="E972" t="n">
-        <v>-992921569</v>
+        <v>992921569</v>
       </c>
       <c r="F972" t="inlineStr">
         <is>
@@ -31622,7 +31622,7 @@
         <v>12400000</v>
       </c>
       <c r="E975" t="n">
-        <v>-1900824036</v>
+        <v>1900824036</v>
       </c>
       <c r="F975" t="inlineStr">
         <is>
@@ -31654,7 +31654,7 @@
         <v>12400000</v>
       </c>
       <c r="E976" t="n">
-        <v>-1432282264</v>
+        <v>1432282264</v>
       </c>
       <c r="F976" t="inlineStr">
         <is>
@@ -31686,7 +31686,7 @@
         <v>12400000</v>
       </c>
       <c r="E977" t="n">
-        <v>-1692353208</v>
+        <v>1692353208</v>
       </c>
       <c r="F977" t="inlineStr">
         <is>
@@ -31750,7 +31750,7 @@
         <v>12400000</v>
       </c>
       <c r="E979" t="n">
-        <v>-1454829316</v>
+        <v>1454829316</v>
       </c>
       <c r="F979" t="inlineStr">
         <is>
@@ -31782,7 +31782,7 @@
         <v>12400000</v>
       </c>
       <c r="E980" t="n">
-        <v>-273558005</v>
+        <v>273558005</v>
       </c>
       <c r="F980" t="inlineStr">
         <is>
@@ -31814,7 +31814,7 @@
         <v>12400000</v>
       </c>
       <c r="E981" t="n">
-        <v>-1656273686</v>
+        <v>1656273686</v>
       </c>
       <c r="F981" t="inlineStr">
         <is>
@@ -31846,7 +31846,7 @@
         <v>12400000</v>
       </c>
       <c r="E982" t="n">
-        <v>-906264341</v>
+        <v>906264341</v>
       </c>
       <c r="F982" t="inlineStr">
         <is>
@@ -31878,7 +31878,7 @@
         <v>12400000</v>
       </c>
       <c r="E983" t="n">
-        <v>-848169845</v>
+        <v>848169845</v>
       </c>
       <c r="F983" t="inlineStr">
         <is>
@@ -31910,7 +31910,7 @@
         <v>12400000</v>
       </c>
       <c r="E984" t="n">
-        <v>-277413241</v>
+        <v>277413241</v>
       </c>
       <c r="F984" t="inlineStr">
         <is>
@@ -31942,7 +31942,7 @@
         <v>12400000</v>
       </c>
       <c r="E985" t="n">
-        <v>-1093060266</v>
+        <v>1093060266</v>
       </c>
       <c r="F985" t="inlineStr">
         <is>
@@ -31974,7 +31974,7 @@
         <v>12400000</v>
       </c>
       <c r="E986" t="n">
-        <v>-1979740648</v>
+        <v>1979740648</v>
       </c>
       <c r="F986" t="inlineStr">
         <is>
@@ -32006,7 +32006,7 @@
         <v>12400000</v>
       </c>
       <c r="E987" t="n">
-        <v>-902944769</v>
+        <v>902944769</v>
       </c>
       <c r="F987" t="inlineStr">
         <is>
@@ -32134,7 +32134,7 @@
         <v>12400000</v>
       </c>
       <c r="E991" t="n">
-        <v>-1596528333</v>
+        <v>1596528333</v>
       </c>
       <c r="F991" t="inlineStr">
         <is>
@@ -32230,7 +32230,7 @@
         <v>12300000</v>
       </c>
       <c r="E994" t="n">
-        <v>-2080282993</v>
+        <v>2080282993</v>
       </c>
       <c r="F994" t="inlineStr">
         <is>

</xml_diff>